<commit_message>
Add further collected data
</commit_message>
<xml_diff>
--- a/workflow-analysis-and-rewrite/runtime-analysis-and-rewrite.xlsx
+++ b/workflow-analysis-and-rewrite/runtime-analysis-and-rewrite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wederbn\Desktop\Coding\PlanQK\qprov-content\workflow-analysis-and-rewrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD9DB92-5EF0-464C-A58E-17F25E4FE644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4D46FC-9ECD-4018-B77B-925BD3BB1B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{DFC69C5A-AAD8-407D-8907-336986DC4050}"/>
   </bookViews>
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4836293F-B9CB-4320-909E-74B95BB4C54A}">
   <dimension ref="A1:O351"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="A180" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +603,7 @@
       </c>
       <c r="N4">
         <f>MEDIAN(C102:C151)</f>
-        <v>452</v>
+        <v>483</v>
       </c>
       <c r="O4">
         <f>MEDIAN(D102:D151)</f>
@@ -633,6 +633,10 @@
       <c r="M5">
         <v>4</v>
       </c>
+      <c r="N5">
+        <f>MEDIAN(C152:C201)</f>
+        <v>750.5</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -657,6 +661,10 @@
       <c r="M6">
         <v>5</v>
       </c>
+      <c r="N6">
+        <f>MEDIAN(C202:C251)</f>
+        <v>398.5</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -681,6 +689,10 @@
       <c r="M7">
         <v>6</v>
       </c>
+      <c r="N7">
+        <f>MEDIAN(C252:C301)</f>
+        <v>588</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -705,6 +717,10 @@
       <c r="M8">
         <v>7</v>
       </c>
+      <c r="N8">
+        <f>MEDIAN(C302:C351)</f>
+        <v>733</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -2667,7 +2683,7 @@
         <v>1</v>
       </c>
       <c r="C102" s="3">
-        <v>437</v>
+        <v>557</v>
       </c>
       <c r="D102" s="3">
         <f t="shared" si="1"/>
@@ -2694,7 +2710,7 @@
         <v>2</v>
       </c>
       <c r="C103" s="3">
-        <v>456</v>
+        <v>476</v>
       </c>
       <c r="D103" s="3">
         <f t="shared" si="1"/>
@@ -2802,7 +2818,7 @@
         <v>6</v>
       </c>
       <c r="C107" s="3">
-        <v>448</v>
+        <v>548</v>
       </c>
       <c r="D107" s="3">
         <f t="shared" si="1"/>
@@ -2883,7 +2899,7 @@
         <v>9</v>
       </c>
       <c r="C110" s="3">
-        <v>441</v>
+        <v>461</v>
       </c>
       <c r="D110" s="3">
         <f t="shared" si="1"/>
@@ -2991,7 +3007,7 @@
         <v>13</v>
       </c>
       <c r="C114" s="3">
-        <v>453</v>
+        <v>573</v>
       </c>
       <c r="D114" s="3">
         <f t="shared" si="1"/>
@@ -3045,7 +3061,7 @@
         <v>15</v>
       </c>
       <c r="C116" s="3">
-        <v>466</v>
+        <v>486</v>
       </c>
       <c r="D116" s="3">
         <f t="shared" si="1"/>
@@ -3072,7 +3088,7 @@
         <v>16</v>
       </c>
       <c r="C117" s="3">
-        <v>565</v>
+        <v>585</v>
       </c>
       <c r="D117" s="3">
         <f t="shared" si="1"/>
@@ -3180,7 +3196,7 @@
         <v>20</v>
       </c>
       <c r="C121" s="3">
-        <v>450</v>
+        <v>470</v>
       </c>
       <c r="D121" s="3">
         <f t="shared" si="1"/>
@@ -3288,7 +3304,7 @@
         <v>24</v>
       </c>
       <c r="C125" s="3">
-        <v>455</v>
+        <v>575</v>
       </c>
       <c r="D125" s="3">
         <f t="shared" si="1"/>
@@ -3342,7 +3358,7 @@
         <v>26</v>
       </c>
       <c r="C127" s="3">
-        <v>471</v>
+        <v>571</v>
       </c>
       <c r="D127" s="3">
         <f t="shared" si="1"/>
@@ -3369,7 +3385,7 @@
         <v>27</v>
       </c>
       <c r="C128" s="3">
-        <v>431</v>
+        <v>451</v>
       </c>
       <c r="D128" s="3">
         <f t="shared" si="1"/>
@@ -3396,7 +3412,7 @@
         <v>28</v>
       </c>
       <c r="C129" s="3">
-        <v>417</v>
+        <v>437</v>
       </c>
       <c r="D129" s="3">
         <f t="shared" si="1"/>
@@ -3423,7 +3439,7 @@
         <v>29</v>
       </c>
       <c r="C130" s="3">
-        <v>310</v>
+        <v>450</v>
       </c>
       <c r="D130" s="3">
         <f t="shared" si="1"/>
@@ -3450,7 +3466,7 @@
         <v>30</v>
       </c>
       <c r="C131" s="3">
-        <v>390</v>
+        <v>590</v>
       </c>
       <c r="D131" s="3">
         <f t="shared" ref="D131:D194" si="2">SUM(E131:J131)</f>
@@ -3477,7 +3493,7 @@
         <v>31</v>
       </c>
       <c r="C132" s="3">
-        <v>408</v>
+        <v>548</v>
       </c>
       <c r="D132" s="3">
         <f t="shared" si="2"/>
@@ -3504,7 +3520,7 @@
         <v>32</v>
       </c>
       <c r="C133" s="3">
-        <v>385</v>
+        <v>485</v>
       </c>
       <c r="D133" s="3">
         <f t="shared" si="2"/>
@@ -3531,7 +3547,7 @@
         <v>33</v>
       </c>
       <c r="C134" s="3">
-        <v>439</v>
+        <v>559</v>
       </c>
       <c r="D134" s="3">
         <f t="shared" si="2"/>
@@ -3612,7 +3628,7 @@
         <v>36</v>
       </c>
       <c r="C137" s="3">
-        <v>368</v>
+        <v>408</v>
       </c>
       <c r="D137" s="3">
         <f t="shared" si="2"/>
@@ -3639,7 +3655,7 @@
         <v>37</v>
       </c>
       <c r="C138" s="3">
-        <v>428</v>
+        <v>448</v>
       </c>
       <c r="D138" s="3">
         <f t="shared" si="2"/>
@@ -3666,7 +3682,7 @@
         <v>38</v>
       </c>
       <c r="C139" s="3">
-        <v>389</v>
+        <v>409</v>
       </c>
       <c r="D139" s="3">
         <f t="shared" si="2"/>
@@ -3693,7 +3709,7 @@
         <v>39</v>
       </c>
       <c r="C140" s="3">
-        <v>418</v>
+        <v>538</v>
       </c>
       <c r="D140" s="3">
         <f t="shared" si="2"/>
@@ -3720,7 +3736,7 @@
         <v>40</v>
       </c>
       <c r="C141" s="3">
-        <v>318</v>
+        <v>438</v>
       </c>
       <c r="D141" s="3">
         <f t="shared" si="2"/>
@@ -3747,7 +3763,7 @@
         <v>41</v>
       </c>
       <c r="C142" s="3">
-        <v>410</v>
+        <v>530</v>
       </c>
       <c r="D142" s="3">
         <f t="shared" si="2"/>
@@ -3855,7 +3871,7 @@
         <v>45</v>
       </c>
       <c r="C146" s="3">
-        <v>392</v>
+        <v>492</v>
       </c>
       <c r="D146" s="3">
         <f t="shared" si="2"/>
@@ -3882,7 +3898,7 @@
         <v>46</v>
       </c>
       <c r="C147" s="3">
-        <v>454</v>
+        <v>474</v>
       </c>
       <c r="D147" s="3">
         <f t="shared" si="2"/>
@@ -3936,7 +3952,7 @@
         <v>48</v>
       </c>
       <c r="C149" s="3">
-        <v>383</v>
+        <v>523</v>
       </c>
       <c r="D149" s="3">
         <f t="shared" si="2"/>
@@ -3963,7 +3979,7 @@
         <v>49</v>
       </c>
       <c r="C150" s="3">
-        <v>442</v>
+        <v>562</v>
       </c>
       <c r="D150" s="3">
         <f t="shared" si="2"/>
@@ -3990,7 +4006,7 @@
         <v>50</v>
       </c>
       <c r="C151" s="3">
-        <v>421</v>
+        <v>541</v>
       </c>
       <c r="D151" s="3">
         <f t="shared" si="2"/>
@@ -4016,6 +4032,9 @@
       <c r="B152">
         <v>1</v>
       </c>
+      <c r="C152" s="3">
+        <v>740</v>
+      </c>
       <c r="D152" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4028,6 +4047,9 @@
       <c r="B153">
         <v>2</v>
       </c>
+      <c r="C153" s="3">
+        <v>696</v>
+      </c>
       <c r="D153" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4040,6 +4062,9 @@
       <c r="B154">
         <v>3</v>
       </c>
+      <c r="C154" s="3">
+        <v>775</v>
+      </c>
       <c r="D154" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4052,6 +4077,9 @@
       <c r="B155">
         <v>4</v>
       </c>
+      <c r="C155" s="3">
+        <v>755</v>
+      </c>
       <c r="D155" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4064,6 +4092,9 @@
       <c r="B156">
         <v>5</v>
       </c>
+      <c r="C156" s="3">
+        <v>750</v>
+      </c>
       <c r="D156" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4076,6 +4107,9 @@
       <c r="B157">
         <v>6</v>
       </c>
+      <c r="C157" s="3">
+        <v>679</v>
+      </c>
       <c r="D157" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4088,6 +4122,9 @@
       <c r="B158">
         <v>7</v>
       </c>
+      <c r="C158" s="3">
+        <v>692</v>
+      </c>
       <c r="D158" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4100,6 +4137,9 @@
       <c r="B159">
         <v>8</v>
       </c>
+      <c r="C159" s="3">
+        <v>695</v>
+      </c>
       <c r="D159" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4112,6 +4152,9 @@
       <c r="B160">
         <v>9</v>
       </c>
+      <c r="C160" s="3">
+        <v>804</v>
+      </c>
       <c r="D160" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4124,6 +4167,9 @@
       <c r="B161">
         <v>10</v>
       </c>
+      <c r="C161" s="3">
+        <v>794</v>
+      </c>
       <c r="D161" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4136,6 +4182,9 @@
       <c r="B162">
         <v>11</v>
       </c>
+      <c r="C162" s="3">
+        <v>783</v>
+      </c>
       <c r="D162" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4148,6 +4197,9 @@
       <c r="B163">
         <v>12</v>
       </c>
+      <c r="C163" s="3">
+        <v>736</v>
+      </c>
       <c r="D163" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4160,6 +4212,9 @@
       <c r="B164">
         <v>13</v>
       </c>
+      <c r="C164" s="3">
+        <v>781</v>
+      </c>
       <c r="D164" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4172,6 +4227,9 @@
       <c r="B165">
         <v>14</v>
       </c>
+      <c r="C165" s="3">
+        <v>721</v>
+      </c>
       <c r="D165" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4184,6 +4242,9 @@
       <c r="B166">
         <v>15</v>
       </c>
+      <c r="C166" s="3">
+        <v>725</v>
+      </c>
       <c r="D166" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4196,6 +4257,9 @@
       <c r="B167">
         <v>16</v>
       </c>
+      <c r="C167" s="3">
+        <v>730</v>
+      </c>
       <c r="D167" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4208,6 +4272,9 @@
       <c r="B168">
         <v>17</v>
       </c>
+      <c r="C168" s="3">
+        <v>743</v>
+      </c>
       <c r="D168" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4220,6 +4287,9 @@
       <c r="B169">
         <v>18</v>
       </c>
+      <c r="C169" s="3">
+        <v>779</v>
+      </c>
       <c r="D169" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4232,6 +4302,9 @@
       <c r="B170">
         <v>19</v>
       </c>
+      <c r="C170" s="3">
+        <v>706</v>
+      </c>
       <c r="D170" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4244,6 +4317,9 @@
       <c r="B171">
         <v>20</v>
       </c>
+      <c r="C171" s="3">
+        <v>710</v>
+      </c>
       <c r="D171" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4256,6 +4332,9 @@
       <c r="B172">
         <v>21</v>
       </c>
+      <c r="C172" s="3">
+        <v>774</v>
+      </c>
       <c r="D172" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4268,6 +4347,9 @@
       <c r="B173">
         <v>22</v>
       </c>
+      <c r="C173" s="3">
+        <v>743</v>
+      </c>
       <c r="D173" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4280,6 +4362,9 @@
       <c r="B174">
         <v>23</v>
       </c>
+      <c r="C174" s="3">
+        <v>673</v>
+      </c>
       <c r="D174" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4292,6 +4377,9 @@
       <c r="B175">
         <v>24</v>
       </c>
+      <c r="C175" s="3">
+        <v>638</v>
+      </c>
       <c r="D175" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4304,6 +4392,9 @@
       <c r="B176">
         <v>25</v>
       </c>
+      <c r="C176" s="3">
+        <v>741</v>
+      </c>
       <c r="D176" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4316,6 +4407,9 @@
       <c r="B177">
         <v>26</v>
       </c>
+      <c r="C177" s="3">
+        <v>704</v>
+      </c>
       <c r="D177" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4328,6 +4422,9 @@
       <c r="B178">
         <v>27</v>
       </c>
+      <c r="C178" s="3">
+        <v>796</v>
+      </c>
       <c r="D178" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4340,6 +4437,9 @@
       <c r="B179">
         <v>28</v>
       </c>
+      <c r="C179" s="3">
+        <v>793</v>
+      </c>
       <c r="D179" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4352,6 +4452,9 @@
       <c r="B180">
         <v>29</v>
       </c>
+      <c r="C180" s="3">
+        <v>796</v>
+      </c>
       <c r="D180" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4364,6 +4467,9 @@
       <c r="B181">
         <v>30</v>
       </c>
+      <c r="C181" s="3">
+        <v>776</v>
+      </c>
       <c r="D181" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4376,6 +4482,9 @@
       <c r="B182">
         <v>31</v>
       </c>
+      <c r="C182" s="3">
+        <v>810</v>
+      </c>
       <c r="D182" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4388,6 +4497,9 @@
       <c r="B183">
         <v>32</v>
       </c>
+      <c r="C183" s="3">
+        <v>830</v>
+      </c>
       <c r="D183" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4400,6 +4512,9 @@
       <c r="B184">
         <v>33</v>
       </c>
+      <c r="C184" s="3">
+        <v>783</v>
+      </c>
       <c r="D184" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4412,6 +4527,9 @@
       <c r="B185">
         <v>34</v>
       </c>
+      <c r="C185" s="3">
+        <v>821</v>
+      </c>
       <c r="D185" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4424,6 +4542,9 @@
       <c r="B186">
         <v>35</v>
       </c>
+      <c r="C186" s="3">
+        <v>757</v>
+      </c>
       <c r="D186" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4436,6 +4557,9 @@
       <c r="B187">
         <v>36</v>
       </c>
+      <c r="C187" s="3">
+        <v>751</v>
+      </c>
       <c r="D187" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4448,6 +4572,9 @@
       <c r="B188">
         <v>37</v>
       </c>
+      <c r="C188" s="3">
+        <v>792</v>
+      </c>
       <c r="D188" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4460,6 +4587,9 @@
       <c r="B189">
         <v>38</v>
       </c>
+      <c r="C189" s="3">
+        <v>779</v>
+      </c>
       <c r="D189" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4472,6 +4602,9 @@
       <c r="B190">
         <v>39</v>
       </c>
+      <c r="C190" s="3">
+        <v>780</v>
+      </c>
       <c r="D190" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4484,6 +4617,9 @@
       <c r="B191">
         <v>40</v>
       </c>
+      <c r="C191" s="3">
+        <v>662</v>
+      </c>
       <c r="D191" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4496,6 +4632,9 @@
       <c r="B192">
         <v>41</v>
       </c>
+      <c r="C192" s="3">
+        <v>865</v>
+      </c>
       <c r="D192" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4508,6 +4647,9 @@
       <c r="B193">
         <v>42</v>
       </c>
+      <c r="C193" s="3">
+        <v>797</v>
+      </c>
       <c r="D193" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4520,6 +4662,9 @@
       <c r="B194">
         <v>43</v>
       </c>
+      <c r="C194" s="3">
+        <v>720</v>
+      </c>
       <c r="D194" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4532,6 +4677,9 @@
       <c r="B195">
         <v>44</v>
       </c>
+      <c r="C195" s="3">
+        <v>730</v>
+      </c>
       <c r="D195" s="3">
         <f t="shared" ref="D195:D258" si="3">SUM(E195:J195)</f>
         <v>0</v>
@@ -4544,6 +4692,9 @@
       <c r="B196">
         <v>45</v>
       </c>
+      <c r="C196" s="3">
+        <v>733</v>
+      </c>
       <c r="D196" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4556,6 +4707,9 @@
       <c r="B197">
         <v>46</v>
       </c>
+      <c r="C197" s="3">
+        <v>707</v>
+      </c>
       <c r="D197" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4568,6 +4722,9 @@
       <c r="B198">
         <v>47</v>
       </c>
+      <c r="C198" s="3">
+        <v>797</v>
+      </c>
       <c r="D198" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4580,6 +4737,9 @@
       <c r="B199">
         <v>48</v>
       </c>
+      <c r="C199" s="3">
+        <v>782</v>
+      </c>
       <c r="D199" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4592,6 +4752,9 @@
       <c r="B200">
         <v>49</v>
       </c>
+      <c r="C200" s="3">
+        <v>657</v>
+      </c>
       <c r="D200" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4604,6 +4767,9 @@
       <c r="B201">
         <v>50</v>
       </c>
+      <c r="C201" s="3">
+        <v>716</v>
+      </c>
       <c r="D201" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4616,6 +4782,9 @@
       <c r="B202">
         <v>1</v>
       </c>
+      <c r="C202" s="3">
+        <v>351</v>
+      </c>
       <c r="D202" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4628,6 +4797,9 @@
       <c r="B203">
         <v>2</v>
       </c>
+      <c r="C203" s="3">
+        <v>338</v>
+      </c>
       <c r="D203" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4640,6 +4812,9 @@
       <c r="B204">
         <v>3</v>
       </c>
+      <c r="C204" s="3">
+        <v>416</v>
+      </c>
       <c r="D204" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4652,6 +4827,9 @@
       <c r="B205">
         <v>4</v>
       </c>
+      <c r="C205" s="3">
+        <v>390</v>
+      </c>
       <c r="D205" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4664,6 +4842,9 @@
       <c r="B206">
         <v>5</v>
       </c>
+      <c r="C206" s="3">
+        <v>454</v>
+      </c>
       <c r="D206" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4676,6 +4857,9 @@
       <c r="B207">
         <v>6</v>
       </c>
+      <c r="C207" s="3">
+        <v>453</v>
+      </c>
       <c r="D207" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4688,6 +4872,9 @@
       <c r="B208">
         <v>7</v>
       </c>
+      <c r="C208" s="3">
+        <v>307</v>
+      </c>
       <c r="D208" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4700,6 +4887,9 @@
       <c r="B209">
         <v>8</v>
       </c>
+      <c r="C209" s="3">
+        <v>305</v>
+      </c>
       <c r="D209" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4712,6 +4902,9 @@
       <c r="B210">
         <v>9</v>
       </c>
+      <c r="C210" s="3">
+        <v>308</v>
+      </c>
       <c r="D210" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4724,6 +4917,9 @@
       <c r="B211">
         <v>10</v>
       </c>
+      <c r="C211" s="3">
+        <v>415</v>
+      </c>
       <c r="D211" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4736,6 +4932,9 @@
       <c r="B212">
         <v>11</v>
       </c>
+      <c r="C212" s="3">
+        <v>405</v>
+      </c>
       <c r="D212" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4748,6 +4947,9 @@
       <c r="B213">
         <v>12</v>
       </c>
+      <c r="C213" s="3">
+        <v>370</v>
+      </c>
       <c r="D213" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4760,6 +4962,9 @@
       <c r="B214">
         <v>13</v>
       </c>
+      <c r="C214" s="3">
+        <v>425</v>
+      </c>
       <c r="D214" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4772,6 +4977,9 @@
       <c r="B215">
         <v>14</v>
       </c>
+      <c r="C215" s="3">
+        <v>395</v>
+      </c>
       <c r="D215" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4784,6 +4992,9 @@
       <c r="B216">
         <v>15</v>
       </c>
+      <c r="C216" s="3">
+        <v>987</v>
+      </c>
       <c r="D216" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4796,6 +5007,9 @@
       <c r="B217">
         <v>16</v>
       </c>
+      <c r="C217" s="3">
+        <v>394</v>
+      </c>
       <c r="D217" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4808,6 +5022,9 @@
       <c r="B218">
         <v>17</v>
       </c>
+      <c r="C218" s="3">
+        <v>424</v>
+      </c>
       <c r="D218" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4820,6 +5037,9 @@
       <c r="B219">
         <v>18</v>
       </c>
+      <c r="C219" s="3">
+        <v>399</v>
+      </c>
       <c r="D219" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4832,6 +5052,9 @@
       <c r="B220">
         <v>19</v>
       </c>
+      <c r="C220" s="3">
+        <v>396</v>
+      </c>
       <c r="D220" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4844,6 +5067,9 @@
       <c r="B221">
         <v>20</v>
       </c>
+      <c r="C221" s="3">
+        <v>401</v>
+      </c>
       <c r="D221" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4856,6 +5082,9 @@
       <c r="B222">
         <v>21</v>
       </c>
+      <c r="C222" s="3">
+        <v>398</v>
+      </c>
       <c r="D222" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4868,6 +5097,9 @@
       <c r="B223">
         <v>22</v>
       </c>
+      <c r="C223" s="3">
+        <v>435</v>
+      </c>
       <c r="D223" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4880,6 +5112,9 @@
       <c r="B224">
         <v>23</v>
       </c>
+      <c r="C224" s="3">
+        <v>439</v>
+      </c>
       <c r="D224" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4892,6 +5127,9 @@
       <c r="B225">
         <v>24</v>
       </c>
+      <c r="C225" s="3">
+        <v>417</v>
+      </c>
       <c r="D225" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4904,6 +5142,9 @@
       <c r="B226">
         <v>25</v>
       </c>
+      <c r="C226" s="3">
+        <v>418</v>
+      </c>
       <c r="D226" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4916,6 +5157,9 @@
       <c r="B227">
         <v>26</v>
       </c>
+      <c r="C227" s="3">
+        <v>402</v>
+      </c>
       <c r="D227" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4928,6 +5172,9 @@
       <c r="B228">
         <v>27</v>
       </c>
+      <c r="C228" s="3">
+        <v>446</v>
+      </c>
       <c r="D228" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4940,6 +5187,9 @@
       <c r="B229">
         <v>28</v>
       </c>
+      <c r="C229" s="3">
+        <v>477</v>
+      </c>
       <c r="D229" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4952,6 +5202,9 @@
       <c r="B230">
         <v>29</v>
       </c>
+      <c r="C230" s="3">
+        <v>470</v>
+      </c>
       <c r="D230" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4964,6 +5217,9 @@
       <c r="B231">
         <v>30</v>
       </c>
+      <c r="C231" s="3">
+        <v>464</v>
+      </c>
       <c r="D231" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4976,6 +5232,9 @@
       <c r="B232">
         <v>31</v>
       </c>
+      <c r="C232" s="3">
+        <v>435</v>
+      </c>
       <c r="D232" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4988,6 +5247,9 @@
       <c r="B233">
         <v>32</v>
       </c>
+      <c r="C233" s="3">
+        <v>530</v>
+      </c>
       <c r="D233" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5000,6 +5262,9 @@
       <c r="B234">
         <v>33</v>
       </c>
+      <c r="C234" s="3">
+        <v>433</v>
+      </c>
       <c r="D234" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5012,6 +5277,9 @@
       <c r="B235">
         <v>34</v>
       </c>
+      <c r="C235" s="3">
+        <v>469</v>
+      </c>
       <c r="D235" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5024,6 +5292,9 @@
       <c r="B236">
         <v>35</v>
       </c>
+      <c r="C236" s="3">
+        <v>288</v>
+      </c>
       <c r="D236" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5036,6 +5307,9 @@
       <c r="B237">
         <v>36</v>
       </c>
+      <c r="C237" s="3">
+        <v>326</v>
+      </c>
       <c r="D237" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5048,6 +5322,9 @@
       <c r="B238">
         <v>37</v>
       </c>
+      <c r="C238" s="3">
+        <v>326</v>
+      </c>
       <c r="D238" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5060,6 +5337,9 @@
       <c r="B239">
         <v>38</v>
       </c>
+      <c r="C239" s="3">
+        <v>312</v>
+      </c>
       <c r="D239" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5072,6 +5352,9 @@
       <c r="B240">
         <v>39</v>
       </c>
+      <c r="C240" s="3">
+        <v>363</v>
+      </c>
       <c r="D240" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5084,6 +5367,9 @@
       <c r="B241">
         <v>40</v>
       </c>
+      <c r="C241" s="3">
+        <v>331</v>
+      </c>
       <c r="D241" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5096,6 +5382,9 @@
       <c r="B242">
         <v>41</v>
       </c>
+      <c r="C242" s="3">
+        <v>434</v>
+      </c>
       <c r="D242" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5108,6 +5397,9 @@
       <c r="B243">
         <v>42</v>
       </c>
+      <c r="C243" s="3">
+        <v>371</v>
+      </c>
       <c r="D243" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5120,6 +5412,9 @@
       <c r="B244">
         <v>43</v>
       </c>
+      <c r="C244" s="3">
+        <v>386</v>
+      </c>
       <c r="D244" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5132,6 +5427,9 @@
       <c r="B245">
         <v>44</v>
       </c>
+      <c r="C245" s="3">
+        <v>368</v>
+      </c>
       <c r="D245" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5144,6 +5442,9 @@
       <c r="B246">
         <v>45</v>
       </c>
+      <c r="C246" s="3">
+        <v>387</v>
+      </c>
       <c r="D246" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5156,6 +5457,9 @@
       <c r="B247">
         <v>46</v>
       </c>
+      <c r="C247" s="3">
+        <v>360</v>
+      </c>
       <c r="D247" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5168,6 +5472,9 @@
       <c r="B248">
         <v>47</v>
       </c>
+      <c r="C248" s="3">
+        <v>367</v>
+      </c>
       <c r="D248" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5180,6 +5487,9 @@
       <c r="B249">
         <v>48</v>
       </c>
+      <c r="C249" s="3">
+        <v>363</v>
+      </c>
       <c r="D249" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5192,6 +5502,9 @@
       <c r="B250">
         <v>49</v>
       </c>
+      <c r="C250" s="3">
+        <v>381</v>
+      </c>
       <c r="D250" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5204,6 +5517,9 @@
       <c r="B251">
         <v>50</v>
       </c>
+      <c r="C251" s="3">
+        <v>406</v>
+      </c>
       <c r="D251" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5216,6 +5532,9 @@
       <c r="B252">
         <v>1</v>
       </c>
+      <c r="C252" s="3">
+        <v>617</v>
+      </c>
       <c r="D252" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5228,6 +5547,9 @@
       <c r="B253">
         <v>2</v>
       </c>
+      <c r="C253" s="3">
+        <v>605</v>
+      </c>
       <c r="D253" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5240,6 +5562,9 @@
       <c r="B254">
         <v>3</v>
       </c>
+      <c r="C254" s="3">
+        <v>589</v>
+      </c>
       <c r="D254" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5252,6 +5577,9 @@
       <c r="B255">
         <v>4</v>
       </c>
+      <c r="C255" s="3">
+        <v>557</v>
+      </c>
       <c r="D255" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5264,6 +5592,9 @@
       <c r="B256">
         <v>5</v>
       </c>
+      <c r="C256" s="3">
+        <v>574</v>
+      </c>
       <c r="D256" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5276,6 +5607,9 @@
       <c r="B257">
         <v>6</v>
       </c>
+      <c r="C257" s="3">
+        <v>565</v>
+      </c>
       <c r="D257" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5288,6 +5622,9 @@
       <c r="B258">
         <v>7</v>
       </c>
+      <c r="C258" s="3">
+        <v>601</v>
+      </c>
       <c r="D258" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5300,6 +5637,9 @@
       <c r="B259">
         <v>8</v>
       </c>
+      <c r="C259" s="3">
+        <v>585</v>
+      </c>
       <c r="D259" s="3">
         <f t="shared" ref="D259:D322" si="4">SUM(E259:J259)</f>
         <v>0</v>
@@ -5312,6 +5652,9 @@
       <c r="B260">
         <v>9</v>
       </c>
+      <c r="C260" s="3">
+        <v>573</v>
+      </c>
       <c r="D260" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5324,6 +5667,9 @@
       <c r="B261">
         <v>10</v>
       </c>
+      <c r="C261" s="3">
+        <v>649</v>
+      </c>
       <c r="D261" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5336,6 +5682,9 @@
       <c r="B262">
         <v>11</v>
       </c>
+      <c r="C262" s="3">
+        <v>543</v>
+      </c>
       <c r="D262" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5348,6 +5697,9 @@
       <c r="B263">
         <v>12</v>
       </c>
+      <c r="C263" s="3">
+        <v>519</v>
+      </c>
       <c r="D263" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5360,6 +5712,9 @@
       <c r="B264">
         <v>13</v>
       </c>
+      <c r="C264" s="3">
+        <v>580</v>
+      </c>
       <c r="D264" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5372,6 +5727,9 @@
       <c r="B265">
         <v>14</v>
       </c>
+      <c r="C265" s="3">
+        <v>559</v>
+      </c>
       <c r="D265" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5384,6 +5742,9 @@
       <c r="B266">
         <v>15</v>
       </c>
+      <c r="C266" s="3">
+        <v>546</v>
+      </c>
       <c r="D266" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5396,6 +5757,9 @@
       <c r="B267">
         <v>16</v>
       </c>
+      <c r="C267" s="3">
+        <v>580</v>
+      </c>
       <c r="D267" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5408,6 +5772,9 @@
       <c r="B268">
         <v>17</v>
       </c>
+      <c r="C268" s="3">
+        <v>569</v>
+      </c>
       <c r="D268" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5420,6 +5787,9 @@
       <c r="B269">
         <v>18</v>
       </c>
+      <c r="C269" s="3">
+        <v>591</v>
+      </c>
       <c r="D269" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5432,6 +5802,9 @@
       <c r="B270">
         <v>19</v>
       </c>
+      <c r="C270" s="3">
+        <v>539</v>
+      </c>
       <c r="D270" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5444,6 +5817,9 @@
       <c r="B271">
         <v>20</v>
       </c>
+      <c r="C271" s="3">
+        <v>556</v>
+      </c>
       <c r="D271" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5456,6 +5832,9 @@
       <c r="B272">
         <v>21</v>
       </c>
+      <c r="C272" s="3">
+        <v>490</v>
+      </c>
       <c r="D272" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5468,6 +5847,9 @@
       <c r="B273">
         <v>22</v>
       </c>
+      <c r="C273" s="3">
+        <v>595</v>
+      </c>
       <c r="D273" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5480,6 +5862,9 @@
       <c r="B274">
         <v>23</v>
       </c>
+      <c r="C274" s="3">
+        <v>563</v>
+      </c>
       <c r="D274" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5492,6 +5877,9 @@
       <c r="B275">
         <v>24</v>
       </c>
+      <c r="C275" s="3">
+        <v>598</v>
+      </c>
       <c r="D275" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5504,6 +5892,9 @@
       <c r="B276">
         <v>25</v>
       </c>
+      <c r="C276" s="3">
+        <v>574</v>
+      </c>
       <c r="D276" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5516,6 +5907,9 @@
       <c r="B277">
         <v>26</v>
       </c>
+      <c r="C277" s="3">
+        <v>529</v>
+      </c>
       <c r="D277" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5528,6 +5922,9 @@
       <c r="B278">
         <v>27</v>
       </c>
+      <c r="C278" s="3">
+        <v>643</v>
+      </c>
       <c r="D278" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5540,6 +5937,9 @@
       <c r="B279">
         <v>28</v>
       </c>
+      <c r="C279" s="3">
+        <v>581</v>
+      </c>
       <c r="D279" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5552,6 +5952,9 @@
       <c r="B280">
         <v>29</v>
       </c>
+      <c r="C280" s="3">
+        <v>559</v>
+      </c>
       <c r="D280" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5564,6 +5967,9 @@
       <c r="B281">
         <v>30</v>
       </c>
+      <c r="C281" s="3">
+        <v>605</v>
+      </c>
       <c r="D281" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5576,6 +5982,9 @@
       <c r="B282">
         <v>31</v>
       </c>
+      <c r="C282" s="3">
+        <v>618</v>
+      </c>
       <c r="D282" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5588,6 +5997,9 @@
       <c r="B283">
         <v>32</v>
       </c>
+      <c r="C283" s="3">
+        <v>625</v>
+      </c>
       <c r="D283" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5600,6 +6012,9 @@
       <c r="B284">
         <v>33</v>
       </c>
+      <c r="C284" s="3">
+        <v>625</v>
+      </c>
       <c r="D284" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5612,6 +6027,9 @@
       <c r="B285">
         <v>34</v>
       </c>
+      <c r="C285" s="3">
+        <v>621</v>
+      </c>
       <c r="D285" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5624,6 +6042,9 @@
       <c r="B286">
         <v>35</v>
       </c>
+      <c r="C286" s="3">
+        <v>587</v>
+      </c>
       <c r="D286" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5636,6 +6057,9 @@
       <c r="B287">
         <v>36</v>
       </c>
+      <c r="C287" s="3">
+        <v>572</v>
+      </c>
       <c r="D287" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5648,6 +6072,9 @@
       <c r="B288">
         <v>37</v>
       </c>
+      <c r="C288" s="3">
+        <v>619</v>
+      </c>
       <c r="D288" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5660,6 +6087,9 @@
       <c r="B289">
         <v>38</v>
       </c>
+      <c r="C289" s="3">
+        <v>643</v>
+      </c>
       <c r="D289" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5672,6 +6102,9 @@
       <c r="B290">
         <v>39</v>
       </c>
+      <c r="C290" s="3">
+        <v>694</v>
+      </c>
       <c r="D290" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5684,6 +6117,9 @@
       <c r="B291">
         <v>40</v>
       </c>
+      <c r="C291" s="3">
+        <v>445</v>
+      </c>
       <c r="D291" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5696,6 +6132,9 @@
       <c r="B292">
         <v>41</v>
       </c>
+      <c r="C292" s="3">
+        <v>709</v>
+      </c>
       <c r="D292" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5708,6 +6147,9 @@
       <c r="B293">
         <v>42</v>
       </c>
+      <c r="C293" s="3">
+        <v>635</v>
+      </c>
       <c r="D293" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5720,6 +6162,9 @@
       <c r="B294">
         <v>43</v>
       </c>
+      <c r="C294" s="3">
+        <v>658</v>
+      </c>
       <c r="D294" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5732,6 +6177,9 @@
       <c r="B295">
         <v>44</v>
       </c>
+      <c r="C295" s="3">
+        <v>594</v>
+      </c>
       <c r="D295" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5744,6 +6192,9 @@
       <c r="B296">
         <v>45</v>
       </c>
+      <c r="C296" s="3">
+        <v>626</v>
+      </c>
       <c r="D296" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5756,6 +6207,9 @@
       <c r="B297">
         <v>46</v>
       </c>
+      <c r="C297" s="3">
+        <v>640</v>
+      </c>
       <c r="D297" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5768,6 +6222,9 @@
       <c r="B298">
         <v>47</v>
       </c>
+      <c r="C298" s="3">
+        <v>623</v>
+      </c>
       <c r="D298" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5780,6 +6237,9 @@
       <c r="B299">
         <v>48</v>
       </c>
+      <c r="C299" s="3">
+        <v>647</v>
+      </c>
       <c r="D299" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5792,6 +6252,9 @@
       <c r="B300">
         <v>49</v>
       </c>
+      <c r="C300" s="3">
+        <v>485</v>
+      </c>
       <c r="D300" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5804,6 +6267,9 @@
       <c r="B301">
         <v>50</v>
       </c>
+      <c r="C301" s="3">
+        <v>441</v>
+      </c>
       <c r="D301" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5816,6 +6282,9 @@
       <c r="B302">
         <v>1</v>
       </c>
+      <c r="C302" s="3">
+        <v>689</v>
+      </c>
       <c r="D302" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5828,6 +6297,9 @@
       <c r="B303">
         <v>2</v>
       </c>
+      <c r="C303" s="3">
+        <v>714</v>
+      </c>
       <c r="D303" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5840,6 +6312,9 @@
       <c r="B304">
         <v>3</v>
       </c>
+      <c r="C304" s="3">
+        <v>727</v>
+      </c>
       <c r="D304" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5852,6 +6327,9 @@
       <c r="B305">
         <v>4</v>
       </c>
+      <c r="C305" s="3">
+        <v>711</v>
+      </c>
       <c r="D305" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5864,6 +6342,9 @@
       <c r="B306">
         <v>5</v>
       </c>
+      <c r="C306" s="3">
+        <v>710</v>
+      </c>
       <c r="D306" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5876,6 +6357,9 @@
       <c r="B307">
         <v>6</v>
       </c>
+      <c r="C307" s="3">
+        <v>720</v>
+      </c>
       <c r="D307" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5888,6 +6372,9 @@
       <c r="B308">
         <v>7</v>
       </c>
+      <c r="C308" s="3">
+        <v>733</v>
+      </c>
       <c r="D308" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5900,6 +6387,9 @@
       <c r="B309">
         <v>8</v>
       </c>
+      <c r="C309" s="3">
+        <v>784</v>
+      </c>
       <c r="D309" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5912,6 +6402,9 @@
       <c r="B310">
         <v>9</v>
       </c>
+      <c r="C310" s="3">
+        <v>659</v>
+      </c>
       <c r="D310" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5924,6 +6417,9 @@
       <c r="B311">
         <v>10</v>
       </c>
+      <c r="C311" s="3">
+        <v>657</v>
+      </c>
       <c r="D311" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5936,6 +6432,9 @@
       <c r="B312">
         <v>11</v>
       </c>
+      <c r="C312" s="3">
+        <v>631</v>
+      </c>
       <c r="D312" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5948,6 +6447,9 @@
       <c r="B313">
         <v>12</v>
       </c>
+      <c r="C313" s="3">
+        <v>661</v>
+      </c>
       <c r="D313" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5960,6 +6462,9 @@
       <c r="B314">
         <v>13</v>
       </c>
+      <c r="C314" s="3">
+        <v>655</v>
+      </c>
       <c r="D314" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5972,6 +6477,9 @@
       <c r="B315">
         <v>14</v>
       </c>
+      <c r="C315" s="3">
+        <v>656</v>
+      </c>
       <c r="D315" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5984,6 +6492,9 @@
       <c r="B316">
         <v>15</v>
       </c>
+      <c r="C316" s="3">
+        <v>640</v>
+      </c>
       <c r="D316" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5996,6 +6507,9 @@
       <c r="B317">
         <v>16</v>
       </c>
+      <c r="C317" s="3">
+        <v>642</v>
+      </c>
       <c r="D317" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -6008,6 +6522,9 @@
       <c r="B318">
         <v>17</v>
       </c>
+      <c r="C318" s="3">
+        <v>659</v>
+      </c>
       <c r="D318" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -6020,6 +6537,9 @@
       <c r="B319">
         <v>18</v>
       </c>
+      <c r="C319" s="3">
+        <v>654</v>
+      </c>
       <c r="D319" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -6032,6 +6552,9 @@
       <c r="B320">
         <v>19</v>
       </c>
+      <c r="C320" s="3">
+        <v>644</v>
+      </c>
       <c r="D320" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -6044,6 +6567,9 @@
       <c r="B321">
         <v>20</v>
       </c>
+      <c r="C321" s="3">
+        <v>701</v>
+      </c>
       <c r="D321" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -6056,6 +6582,9 @@
       <c r="B322">
         <v>21</v>
       </c>
+      <c r="C322" s="3">
+        <v>673</v>
+      </c>
       <c r="D322" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -6068,6 +6597,9 @@
       <c r="B323">
         <v>22</v>
       </c>
+      <c r="C323" s="3">
+        <v>708</v>
+      </c>
       <c r="D323" s="3">
         <f t="shared" ref="D323:D351" si="5">SUM(E323:J323)</f>
         <v>0</v>
@@ -6080,6 +6612,9 @@
       <c r="B324">
         <v>23</v>
       </c>
+      <c r="C324" s="3">
+        <v>754</v>
+      </c>
       <c r="D324" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6092,6 +6627,9 @@
       <c r="B325">
         <v>24</v>
       </c>
+      <c r="C325" s="3">
+        <v>852</v>
+      </c>
       <c r="D325" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6104,6 +6642,9 @@
       <c r="B326">
         <v>25</v>
       </c>
+      <c r="C326" s="3">
+        <v>879</v>
+      </c>
       <c r="D326" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6116,6 +6657,9 @@
       <c r="B327">
         <v>26</v>
       </c>
+      <c r="C327" s="3">
+        <v>892</v>
+      </c>
       <c r="D327" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6128,6 +6672,9 @@
       <c r="B328">
         <v>27</v>
       </c>
+      <c r="C328" s="3">
+        <v>729</v>
+      </c>
       <c r="D328" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6140,6 +6687,9 @@
       <c r="B329">
         <v>28</v>
       </c>
+      <c r="C329" s="3">
+        <v>723</v>
+      </c>
       <c r="D329" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6152,6 +6702,9 @@
       <c r="B330">
         <v>29</v>
       </c>
+      <c r="C330" s="3">
+        <v>739</v>
+      </c>
       <c r="D330" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6164,6 +6717,9 @@
       <c r="B331">
         <v>30</v>
       </c>
+      <c r="C331" s="3">
+        <v>713</v>
+      </c>
       <c r="D331" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6176,6 +6732,9 @@
       <c r="B332">
         <v>31</v>
       </c>
+      <c r="C332" s="3">
+        <v>837</v>
+      </c>
       <c r="D332" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6188,6 +6747,9 @@
       <c r="B333">
         <v>32</v>
       </c>
+      <c r="C333" s="3">
+        <v>776</v>
+      </c>
       <c r="D333" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6200,6 +6762,9 @@
       <c r="B334">
         <v>33</v>
       </c>
+      <c r="C334" s="3">
+        <v>764</v>
+      </c>
       <c r="D334" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6212,6 +6777,9 @@
       <c r="B335">
         <v>34</v>
       </c>
+      <c r="C335" s="3">
+        <v>733</v>
+      </c>
       <c r="D335" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6224,6 +6792,9 @@
       <c r="B336">
         <v>35</v>
       </c>
+      <c r="C336" s="3">
+        <v>767</v>
+      </c>
       <c r="D336" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6236,6 +6807,9 @@
       <c r="B337">
         <v>36</v>
       </c>
+      <c r="C337" s="3">
+        <v>785</v>
+      </c>
       <c r="D337" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6248,6 +6822,9 @@
       <c r="B338">
         <v>37</v>
       </c>
+      <c r="C338" s="3">
+        <v>885</v>
+      </c>
       <c r="D338" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6260,6 +6837,9 @@
       <c r="B339">
         <v>38</v>
       </c>
+      <c r="C339" s="3">
+        <v>778</v>
+      </c>
       <c r="D339" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6272,6 +6852,9 @@
       <c r="B340">
         <v>39</v>
       </c>
+      <c r="C340" s="3">
+        <v>784</v>
+      </c>
       <c r="D340" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6284,6 +6867,9 @@
       <c r="B341">
         <v>40</v>
       </c>
+      <c r="C341" s="3">
+        <v>788</v>
+      </c>
       <c r="D341" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6296,6 +6882,9 @@
       <c r="B342">
         <v>41</v>
       </c>
+      <c r="C342" s="3">
+        <v>767</v>
+      </c>
       <c r="D342" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6308,6 +6897,9 @@
       <c r="B343">
         <v>42</v>
       </c>
+      <c r="C343" s="3">
+        <v>793</v>
+      </c>
       <c r="D343" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6320,6 +6912,9 @@
       <c r="B344">
         <v>43</v>
       </c>
+      <c r="C344" s="3">
+        <v>812</v>
+      </c>
       <c r="D344" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6332,6 +6927,9 @@
       <c r="B345">
         <v>44</v>
       </c>
+      <c r="C345" s="3">
+        <v>801</v>
+      </c>
       <c r="D345" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6344,6 +6942,9 @@
       <c r="B346">
         <v>45</v>
       </c>
+      <c r="C346" s="3">
+        <v>837</v>
+      </c>
       <c r="D346" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6356,6 +6957,9 @@
       <c r="B347">
         <v>46</v>
       </c>
+      <c r="C347" s="3">
+        <v>858</v>
+      </c>
       <c r="D347" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6368,6 +6972,9 @@
       <c r="B348">
         <v>47</v>
       </c>
+      <c r="C348" s="3">
+        <v>796</v>
+      </c>
       <c r="D348" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6380,6 +6987,9 @@
       <c r="B349">
         <v>48</v>
       </c>
+      <c r="C349" s="3">
+        <v>720</v>
+      </c>
       <c r="D349" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6392,6 +7002,9 @@
       <c r="B350">
         <v>49</v>
       </c>
+      <c r="C350" s="3">
+        <v>792</v>
+      </c>
       <c r="D350" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6403,6 +7016,9 @@
       </c>
       <c r="B351">
         <v>50</v>
+      </c>
+      <c r="C351" s="3">
+        <v>743</v>
       </c>
       <c r="D351" s="3">
         <f t="shared" si="5"/>
@@ -6413,7 +7029,7 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="N2:N3" formulaRange="1"/>
+    <ignoredError sqref="N2:N6 N7:N8" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add data for workflow 4
</commit_message>
<xml_diff>
--- a/workflow-analysis-and-rewrite/runtime-analysis-and-rewrite.xlsx
+++ b/workflow-analysis-and-rewrite/runtime-analysis-and-rewrite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wederbn\Desktop\Coding\PlanQK\qprov-content\workflow-analysis-and-rewrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4D46FC-9ECD-4018-B77B-925BD3BB1B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EE2F30-3963-4F72-A19A-F6A7E464048D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{DFC69C5A-AAD8-407D-8907-336986DC4050}"/>
   </bookViews>
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4836293F-B9CB-4320-909E-74B95BB4C54A}">
   <dimension ref="A1:O351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="C193" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,6 +637,10 @@
         <f>MEDIAN(C152:C201)</f>
         <v>750.5</v>
       </c>
+      <c r="O5">
+        <f>MEDIAN(D152:D201)</f>
+        <v>323449.5</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -3836,7 +3840,7 @@
         <v>46707</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>3</v>
       </c>
@@ -3863,7 +3867,7 @@
         <v>47997</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>3</v>
       </c>
@@ -3890,7 +3894,7 @@
         <v>48959</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>3</v>
       </c>
@@ -3917,7 +3921,7 @@
         <v>39722</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>3</v>
       </c>
@@ -3944,7 +3948,7 @@
         <v>44973</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>3</v>
       </c>
@@ -3971,7 +3975,7 @@
         <v>40086</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>3</v>
       </c>
@@ -3998,7 +4002,7 @@
         <v>49688</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>3</v>
       </c>
@@ -4025,7 +4029,7 @@
         <v>45001</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>4</v>
       </c>
@@ -4037,10 +4041,28 @@
       </c>
       <c r="D152" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+        <v>318431</v>
+      </c>
+      <c r="E152" s="3">
+        <v>67766</v>
+      </c>
+      <c r="F152" s="3">
+        <v>43589</v>
+      </c>
+      <c r="G152" s="3">
+        <v>63784</v>
+      </c>
+      <c r="H152" s="3">
+        <v>42677</v>
+      </c>
+      <c r="I152" s="3">
+        <v>58967</v>
+      </c>
+      <c r="J152" s="3">
+        <v>41648</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>4</v>
       </c>
@@ -4052,10 +4074,28 @@
       </c>
       <c r="D153" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+        <v>326876</v>
+      </c>
+      <c r="E153" s="3">
+        <v>62901</v>
+      </c>
+      <c r="F153" s="3">
+        <v>47232</v>
+      </c>
+      <c r="G153" s="3">
+        <v>67590</v>
+      </c>
+      <c r="H153" s="3">
+        <v>44254</v>
+      </c>
+      <c r="I153" s="3">
+        <v>66165</v>
+      </c>
+      <c r="J153" s="3">
+        <v>38734</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>4</v>
       </c>
@@ -4067,10 +4107,28 @@
       </c>
       <c r="D154" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+        <v>319307</v>
+      </c>
+      <c r="E154" s="3">
+        <v>61376</v>
+      </c>
+      <c r="F154" s="3">
+        <v>42644</v>
+      </c>
+      <c r="G154" s="3">
+        <v>61079</v>
+      </c>
+      <c r="H154" s="3">
+        <v>45646</v>
+      </c>
+      <c r="I154" s="3">
+        <v>61483</v>
+      </c>
+      <c r="J154" s="3">
+        <v>47079</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>4</v>
       </c>
@@ -4082,10 +4140,28 @@
       </c>
       <c r="D155" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+        <v>327420</v>
+      </c>
+      <c r="E155" s="3">
+        <v>67732</v>
+      </c>
+      <c r="F155" s="3">
+        <v>46489</v>
+      </c>
+      <c r="G155" s="3">
+        <v>68431</v>
+      </c>
+      <c r="H155" s="3">
+        <v>39639</v>
+      </c>
+      <c r="I155" s="3">
+        <v>62397</v>
+      </c>
+      <c r="J155" s="3">
+        <v>42732</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>4</v>
       </c>
@@ -4097,10 +4173,28 @@
       </c>
       <c r="D156" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+        <v>342226</v>
+      </c>
+      <c r="E156" s="3">
+        <v>70829</v>
+      </c>
+      <c r="F156" s="3">
+        <v>50610</v>
+      </c>
+      <c r="G156" s="3">
+        <v>70044</v>
+      </c>
+      <c r="H156" s="3">
+        <v>38846</v>
+      </c>
+      <c r="I156" s="3">
+        <v>69791</v>
+      </c>
+      <c r="J156" s="3">
+        <v>42106</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>4</v>
       </c>
@@ -4112,10 +4206,28 @@
       </c>
       <c r="D157" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+        <v>322419</v>
+      </c>
+      <c r="E157" s="3">
+        <v>62453</v>
+      </c>
+      <c r="F157" s="3">
+        <v>41179</v>
+      </c>
+      <c r="G157" s="3">
+        <v>69133</v>
+      </c>
+      <c r="H157" s="3">
+        <v>39414</v>
+      </c>
+      <c r="I157" s="3">
+        <v>64935</v>
+      </c>
+      <c r="J157" s="3">
+        <v>45305</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>4</v>
       </c>
@@ -4127,10 +4239,28 @@
       </c>
       <c r="D158" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+        <v>322856</v>
+      </c>
+      <c r="E158" s="3">
+        <v>60894</v>
+      </c>
+      <c r="F158" s="3">
+        <v>42976</v>
+      </c>
+      <c r="G158" s="3">
+        <v>60803</v>
+      </c>
+      <c r="H158" s="3">
+        <v>39885</v>
+      </c>
+      <c r="I158" s="3">
+        <v>67470</v>
+      </c>
+      <c r="J158" s="3">
+        <v>50828</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>4</v>
       </c>
@@ -4142,10 +4272,28 @@
       </c>
       <c r="D159" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+        <v>325193</v>
+      </c>
+      <c r="E159" s="3">
+        <v>61957</v>
+      </c>
+      <c r="F159" s="3">
+        <v>41336</v>
+      </c>
+      <c r="G159" s="3">
+        <v>65290</v>
+      </c>
+      <c r="H159" s="3">
+        <v>43202</v>
+      </c>
+      <c r="I159" s="3">
+        <v>69823</v>
+      </c>
+      <c r="J159" s="3">
+        <v>43585</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>4</v>
       </c>
@@ -4157,10 +4305,28 @@
       </c>
       <c r="D160" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+        <v>324749</v>
+      </c>
+      <c r="E160" s="3">
+        <v>63885</v>
+      </c>
+      <c r="F160" s="3">
+        <v>42682</v>
+      </c>
+      <c r="G160" s="3">
+        <v>67768</v>
+      </c>
+      <c r="H160" s="3">
+        <v>39551</v>
+      </c>
+      <c r="I160" s="3">
+        <v>65062</v>
+      </c>
+      <c r="J160" s="3">
+        <v>45801</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>4</v>
       </c>
@@ -4172,10 +4338,28 @@
       </c>
       <c r="D161" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+        <v>327033</v>
+      </c>
+      <c r="E161" s="3">
+        <v>60922</v>
+      </c>
+      <c r="F161" s="3">
+        <v>39236</v>
+      </c>
+      <c r="G161" s="3">
+        <v>65673</v>
+      </c>
+      <c r="H161" s="3">
+        <v>50538</v>
+      </c>
+      <c r="I161" s="3">
+        <v>64085</v>
+      </c>
+      <c r="J161" s="3">
+        <v>46579</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>4</v>
       </c>
@@ -4187,10 +4371,28 @@
       </c>
       <c r="D162" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+        <v>332331</v>
+      </c>
+      <c r="E162" s="3">
+        <v>65773</v>
+      </c>
+      <c r="F162" s="3">
+        <v>45481</v>
+      </c>
+      <c r="G162" s="3">
+        <v>64746</v>
+      </c>
+      <c r="H162" s="3">
+        <v>46904</v>
+      </c>
+      <c r="I162" s="3">
+        <v>68402</v>
+      </c>
+      <c r="J162" s="3">
+        <v>41025</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>4</v>
       </c>
@@ -4202,10 +4404,28 @@
       </c>
       <c r="D163" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+        <v>329076</v>
+      </c>
+      <c r="E163" s="3">
+        <v>62515</v>
+      </c>
+      <c r="F163" s="3">
+        <v>47615</v>
+      </c>
+      <c r="G163" s="3">
+        <v>64581</v>
+      </c>
+      <c r="H163" s="3">
+        <v>47719</v>
+      </c>
+      <c r="I163" s="3">
+        <v>59753</v>
+      </c>
+      <c r="J163" s="3">
+        <v>46893</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>4</v>
       </c>
@@ -4217,10 +4437,28 @@
       </c>
       <c r="D164" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+        <v>330176</v>
+      </c>
+      <c r="E164" s="3">
+        <v>61199</v>
+      </c>
+      <c r="F164" s="3">
+        <v>50545</v>
+      </c>
+      <c r="G164" s="3">
+        <v>66599</v>
+      </c>
+      <c r="H164" s="3">
+        <v>39774</v>
+      </c>
+      <c r="I164" s="3">
+        <v>66893</v>
+      </c>
+      <c r="J164" s="3">
+        <v>45166</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>4</v>
       </c>
@@ -4232,10 +4470,28 @@
       </c>
       <c r="D165" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+        <v>313993</v>
+      </c>
+      <c r="E165" s="3">
+        <v>69055</v>
+      </c>
+      <c r="F165" s="3">
+        <v>42131</v>
+      </c>
+      <c r="G165" s="3">
+        <v>61662</v>
+      </c>
+      <c r="H165" s="3">
+        <v>42714</v>
+      </c>
+      <c r="I165" s="3">
+        <v>59737</v>
+      </c>
+      <c r="J165" s="3">
+        <v>38694</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>4</v>
       </c>
@@ -4247,10 +4503,28 @@
       </c>
       <c r="D166" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+        <v>333803</v>
+      </c>
+      <c r="E166" s="3">
+        <v>65464</v>
+      </c>
+      <c r="F166" s="3">
+        <v>40138</v>
+      </c>
+      <c r="G166" s="3">
+        <v>68696</v>
+      </c>
+      <c r="H166" s="3">
+        <v>42880</v>
+      </c>
+      <c r="I166" s="3">
+        <v>66018</v>
+      </c>
+      <c r="J166" s="3">
+        <v>50607</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>4</v>
       </c>
@@ -4262,10 +4536,28 @@
       </c>
       <c r="D167" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+        <v>322947</v>
+      </c>
+      <c r="E167" s="3">
+        <v>64148</v>
+      </c>
+      <c r="F167" s="3">
+        <v>40168</v>
+      </c>
+      <c r="G167" s="3">
+        <v>63217</v>
+      </c>
+      <c r="H167" s="3">
+        <v>47552</v>
+      </c>
+      <c r="I167" s="3">
+        <v>69810</v>
+      </c>
+      <c r="J167" s="3">
+        <v>38052</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>4</v>
       </c>
@@ -4277,10 +4569,28 @@
       </c>
       <c r="D168" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+        <v>322372</v>
+      </c>
+      <c r="E168" s="3">
+        <v>66753</v>
+      </c>
+      <c r="F168" s="3">
+        <v>47746</v>
+      </c>
+      <c r="G168" s="3">
+        <v>59167</v>
+      </c>
+      <c r="H168" s="3">
+        <v>39046</v>
+      </c>
+      <c r="I168" s="3">
+        <v>67015</v>
+      </c>
+      <c r="J168" s="3">
+        <v>42645</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>4</v>
       </c>
@@ -4292,10 +4602,28 @@
       </c>
       <c r="D169" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+        <v>323707</v>
+      </c>
+      <c r="E169" s="3">
+        <v>63185</v>
+      </c>
+      <c r="F169" s="3">
+        <v>47603</v>
+      </c>
+      <c r="G169" s="3">
+        <v>69508</v>
+      </c>
+      <c r="H169" s="3">
+        <v>39815</v>
+      </c>
+      <c r="I169" s="3">
+        <v>62653</v>
+      </c>
+      <c r="J169" s="3">
+        <v>40943</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>4</v>
       </c>
@@ -4307,10 +4635,28 @@
       </c>
       <c r="D170" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+        <v>323988</v>
+      </c>
+      <c r="E170" s="3">
+        <v>66249</v>
+      </c>
+      <c r="F170" s="3">
+        <v>38315</v>
+      </c>
+      <c r="G170" s="3">
+        <v>62264</v>
+      </c>
+      <c r="H170" s="3">
+        <v>48878</v>
+      </c>
+      <c r="I170" s="3">
+        <v>65629</v>
+      </c>
+      <c r="J170" s="3">
+        <v>42653</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>4</v>
       </c>
@@ -4322,10 +4668,28 @@
       </c>
       <c r="D171" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+        <v>332555</v>
+      </c>
+      <c r="E171" s="3">
+        <v>61674</v>
+      </c>
+      <c r="F171" s="3">
+        <v>41496</v>
+      </c>
+      <c r="G171" s="3">
+        <v>70709</v>
+      </c>
+      <c r="H171" s="3">
+        <v>44531</v>
+      </c>
+      <c r="I171" s="3">
+        <v>70182</v>
+      </c>
+      <c r="J171" s="3">
+        <v>43963</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>4</v>
       </c>
@@ -4337,10 +4701,28 @@
       </c>
       <c r="D172" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+        <v>308144</v>
+      </c>
+      <c r="E172" s="3">
+        <v>59879</v>
+      </c>
+      <c r="F172" s="3">
+        <v>40640</v>
+      </c>
+      <c r="G172" s="3">
+        <v>66062</v>
+      </c>
+      <c r="H172" s="3">
+        <v>38924</v>
+      </c>
+      <c r="I172" s="3">
+        <v>64120</v>
+      </c>
+      <c r="J172" s="3">
+        <v>38519</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>4</v>
       </c>
@@ -4352,10 +4734,28 @@
       </c>
       <c r="D173" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+        <v>337088</v>
+      </c>
+      <c r="E173" s="3">
+        <v>67136</v>
+      </c>
+      <c r="F173" s="3">
+        <v>40200</v>
+      </c>
+      <c r="G173" s="3">
+        <v>68102</v>
+      </c>
+      <c r="H173" s="3">
+        <v>46507</v>
+      </c>
+      <c r="I173" s="3">
+        <v>68096</v>
+      </c>
+      <c r="J173" s="3">
+        <v>47047</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>4</v>
       </c>
@@ -4367,10 +4767,28 @@
       </c>
       <c r="D174" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+        <v>310829</v>
+      </c>
+      <c r="E174" s="3">
+        <v>59346</v>
+      </c>
+      <c r="F174" s="3">
+        <v>39194</v>
+      </c>
+      <c r="G174" s="3">
+        <v>67176</v>
+      </c>
+      <c r="H174" s="3">
+        <v>39127</v>
+      </c>
+      <c r="I174" s="3">
+        <v>61715</v>
+      </c>
+      <c r="J174" s="3">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>4</v>
       </c>
@@ -4382,10 +4800,28 @@
       </c>
       <c r="D175" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+        <v>326349</v>
+      </c>
+      <c r="E175" s="3">
+        <v>68715</v>
+      </c>
+      <c r="F175" s="3">
+        <v>46302</v>
+      </c>
+      <c r="G175" s="3">
+        <v>61653</v>
+      </c>
+      <c r="H175" s="3">
+        <v>40233</v>
+      </c>
+      <c r="I175" s="3">
+        <v>62751</v>
+      </c>
+      <c r="J175" s="3">
+        <v>46695</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>4</v>
       </c>
@@ -4397,10 +4833,28 @@
       </c>
       <c r="D176" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+        <v>310171</v>
+      </c>
+      <c r="E176" s="3">
+        <v>59067</v>
+      </c>
+      <c r="F176" s="3">
+        <v>40216</v>
+      </c>
+      <c r="G176" s="3">
+        <v>65116</v>
+      </c>
+      <c r="H176" s="3">
+        <v>41694</v>
+      </c>
+      <c r="I176" s="3">
+        <v>59865</v>
+      </c>
+      <c r="J176" s="3">
+        <v>44213</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>4</v>
       </c>
@@ -4412,10 +4866,28 @@
       </c>
       <c r="D177" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+        <v>320103</v>
+      </c>
+      <c r="E177" s="3">
+        <v>59672</v>
+      </c>
+      <c r="F177" s="3">
+        <v>38795</v>
+      </c>
+      <c r="G177" s="3">
+        <v>66122</v>
+      </c>
+      <c r="H177" s="3">
+        <v>44447</v>
+      </c>
+      <c r="I177" s="3">
+        <v>70659</v>
+      </c>
+      <c r="J177" s="3">
+        <v>40408</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>4</v>
       </c>
@@ -4427,10 +4899,28 @@
       </c>
       <c r="D178" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+        <v>319834</v>
+      </c>
+      <c r="E178" s="3">
+        <v>59024</v>
+      </c>
+      <c r="F178" s="3">
+        <v>43284</v>
+      </c>
+      <c r="G178" s="3">
+        <v>61958</v>
+      </c>
+      <c r="H178" s="3">
+        <v>44260</v>
+      </c>
+      <c r="I178" s="3">
+        <v>66259</v>
+      </c>
+      <c r="J178" s="3">
+        <v>45049</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>4</v>
       </c>
@@ -4442,10 +4932,28 @@
       </c>
       <c r="D179" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+        <v>322340</v>
+      </c>
+      <c r="E179" s="3">
+        <v>70014</v>
+      </c>
+      <c r="F179" s="3">
+        <v>45956</v>
+      </c>
+      <c r="G179" s="3">
+        <v>59109</v>
+      </c>
+      <c r="H179" s="3">
+        <v>38276</v>
+      </c>
+      <c r="I179" s="3">
+        <v>65928</v>
+      </c>
+      <c r="J179" s="3">
+        <v>43057</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>4</v>
       </c>
@@ -4457,10 +4965,28 @@
       </c>
       <c r="D180" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+        <v>323192</v>
+      </c>
+      <c r="E180" s="3">
+        <v>62986</v>
+      </c>
+      <c r="F180" s="3">
+        <v>38233</v>
+      </c>
+      <c r="G180" s="3">
+        <v>70648</v>
+      </c>
+      <c r="H180" s="3">
+        <v>44272</v>
+      </c>
+      <c r="I180" s="3">
+        <v>60648</v>
+      </c>
+      <c r="J180" s="3">
+        <v>46405</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>4</v>
       </c>
@@ -4472,10 +4998,28 @@
       </c>
       <c r="D181" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+        <v>319248</v>
+      </c>
+      <c r="E181" s="3">
+        <v>68736</v>
+      </c>
+      <c r="F181" s="3">
+        <v>41299</v>
+      </c>
+      <c r="G181" s="3">
+        <v>60757</v>
+      </c>
+      <c r="H181" s="3">
+        <v>43692</v>
+      </c>
+      <c r="I181" s="3">
+        <v>62533</v>
+      </c>
+      <c r="J181" s="3">
+        <v>42231</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>4</v>
       </c>
@@ -4487,10 +5031,28 @@
       </c>
       <c r="D182" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+        <v>314084</v>
+      </c>
+      <c r="E182" s="3">
+        <v>60223</v>
+      </c>
+      <c r="F182" s="3">
+        <v>45057</v>
+      </c>
+      <c r="G182" s="3">
+        <v>63623</v>
+      </c>
+      <c r="H182" s="3">
+        <v>39607</v>
+      </c>
+      <c r="I182" s="3">
+        <v>61047</v>
+      </c>
+      <c r="J182" s="3">
+        <v>44527</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>4</v>
       </c>
@@ -4502,10 +5064,28 @@
       </c>
       <c r="D183" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+        <v>326163</v>
+      </c>
+      <c r="E183" s="3">
+        <v>59117</v>
+      </c>
+      <c r="F183" s="3">
+        <v>41021</v>
+      </c>
+      <c r="G183" s="3">
+        <v>65547</v>
+      </c>
+      <c r="H183" s="3">
+        <v>42494</v>
+      </c>
+      <c r="I183" s="3">
+        <v>70147</v>
+      </c>
+      <c r="J183" s="3">
+        <v>47837</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>4</v>
       </c>
@@ -4517,10 +5097,28 @@
       </c>
       <c r="D184" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+        <v>328297</v>
+      </c>
+      <c r="E184" s="3">
+        <v>63659</v>
+      </c>
+      <c r="F184" s="3">
+        <v>38506</v>
+      </c>
+      <c r="G184" s="3">
+        <v>66865</v>
+      </c>
+      <c r="H184" s="3">
+        <v>46048</v>
+      </c>
+      <c r="I184" s="3">
+        <v>70934</v>
+      </c>
+      <c r="J184" s="3">
+        <v>42285</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>4</v>
       </c>
@@ -4532,10 +5130,28 @@
       </c>
       <c r="D185" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+        <v>332388</v>
+      </c>
+      <c r="E185" s="3">
+        <v>69586</v>
+      </c>
+      <c r="F185" s="3">
+        <v>44938</v>
+      </c>
+      <c r="G185" s="3">
+        <v>68930</v>
+      </c>
+      <c r="H185" s="3">
+        <v>39926</v>
+      </c>
+      <c r="I185" s="3">
+        <v>65283</v>
+      </c>
+      <c r="J185" s="3">
+        <v>43725</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>4</v>
       </c>
@@ -4547,10 +5163,28 @@
       </c>
       <c r="D186" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+        <v>318080</v>
+      </c>
+      <c r="E186" s="3">
+        <v>59870</v>
+      </c>
+      <c r="F186" s="3">
+        <v>47531</v>
+      </c>
+      <c r="G186" s="3">
+        <v>66187</v>
+      </c>
+      <c r="H186" s="3">
+        <v>38396</v>
+      </c>
+      <c r="I186" s="3">
+        <v>62108</v>
+      </c>
+      <c r="J186" s="3">
+        <v>43988</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>4</v>
       </c>
@@ -4562,10 +5196,28 @@
       </c>
       <c r="D187" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+        <v>315680</v>
+      </c>
+      <c r="E187" s="3">
+        <v>70006</v>
+      </c>
+      <c r="F187" s="3">
+        <v>39851</v>
+      </c>
+      <c r="G187" s="3">
+        <v>59209</v>
+      </c>
+      <c r="H187" s="3">
+        <v>40318</v>
+      </c>
+      <c r="I187" s="3">
+        <v>67821</v>
+      </c>
+      <c r="J187" s="3">
+        <v>38475</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>4</v>
       </c>
@@ -4577,10 +5229,28 @@
       </c>
       <c r="D188" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+        <v>318011</v>
+      </c>
+      <c r="E188" s="3">
+        <v>61405</v>
+      </c>
+      <c r="F188" s="3">
+        <v>43110</v>
+      </c>
+      <c r="G188" s="3">
+        <v>60847</v>
+      </c>
+      <c r="H188" s="3">
+        <v>47826</v>
+      </c>
+      <c r="I188" s="3">
+        <v>65549</v>
+      </c>
+      <c r="J188" s="3">
+        <v>39274</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>4</v>
       </c>
@@ -4592,10 +5262,28 @@
       </c>
       <c r="D189" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+        <v>325182</v>
+      </c>
+      <c r="E189" s="3">
+        <v>67184</v>
+      </c>
+      <c r="F189" s="3">
+        <v>39507</v>
+      </c>
+      <c r="G189" s="3">
+        <v>70149</v>
+      </c>
+      <c r="H189" s="3">
+        <v>45848</v>
+      </c>
+      <c r="I189" s="3">
+        <v>60402</v>
+      </c>
+      <c r="J189" s="3">
+        <v>42092</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>4</v>
       </c>
@@ -4607,10 +5295,28 @@
       </c>
       <c r="D190" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+        <v>335758</v>
+      </c>
+      <c r="E190" s="3">
+        <v>68025</v>
+      </c>
+      <c r="F190" s="3">
+        <v>46897</v>
+      </c>
+      <c r="G190" s="3">
+        <v>66429</v>
+      </c>
+      <c r="H190" s="3">
+        <v>47675</v>
+      </c>
+      <c r="I190" s="3">
+        <v>67622</v>
+      </c>
+      <c r="J190" s="3">
+        <v>39110</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>4</v>
       </c>
@@ -4622,10 +5328,28 @@
       </c>
       <c r="D191" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+        <v>318916</v>
+      </c>
+      <c r="E191" s="3">
+        <v>61223</v>
+      </c>
+      <c r="F191" s="3">
+        <v>40659</v>
+      </c>
+      <c r="G191" s="3">
+        <v>68673</v>
+      </c>
+      <c r="H191" s="3">
+        <v>43226</v>
+      </c>
+      <c r="I191" s="3">
+        <v>65104</v>
+      </c>
+      <c r="J191" s="3">
+        <v>40031</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>4</v>
       </c>
@@ -4637,10 +5361,28 @@
       </c>
       <c r="D192" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+        <v>321999</v>
+      </c>
+      <c r="E192" s="3">
+        <v>64752</v>
+      </c>
+      <c r="F192" s="3">
+        <v>41343</v>
+      </c>
+      <c r="G192" s="3">
+        <v>63776</v>
+      </c>
+      <c r="H192" s="3">
+        <v>46956</v>
+      </c>
+      <c r="I192" s="3">
+        <v>61650</v>
+      </c>
+      <c r="J192" s="3">
+        <v>43522</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>4</v>
       </c>
@@ -4652,10 +5394,28 @@
       </c>
       <c r="D193" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+        <v>324393</v>
+      </c>
+      <c r="E193" s="3">
+        <v>68093</v>
+      </c>
+      <c r="F193" s="3">
+        <v>38708</v>
+      </c>
+      <c r="G193" s="3">
+        <v>67269</v>
+      </c>
+      <c r="H193" s="3">
+        <v>44119</v>
+      </c>
+      <c r="I193" s="3">
+        <v>64025</v>
+      </c>
+      <c r="J193" s="3">
+        <v>42179</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>4</v>
       </c>
@@ -4667,10 +5427,28 @@
       </c>
       <c r="D194" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+        <v>321186</v>
+      </c>
+      <c r="E194" s="3">
+        <v>59894</v>
+      </c>
+      <c r="F194" s="3">
+        <v>41567</v>
+      </c>
+      <c r="G194" s="3">
+        <v>66198</v>
+      </c>
+      <c r="H194" s="3">
+        <v>38560</v>
+      </c>
+      <c r="I194" s="3">
+        <v>69315</v>
+      </c>
+      <c r="J194" s="3">
+        <v>45652</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>4</v>
       </c>
@@ -4682,10 +5460,28 @@
       </c>
       <c r="D195" s="3">
         <f t="shared" ref="D195:D258" si="3">SUM(E195:J195)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+        <v>324035</v>
+      </c>
+      <c r="E195" s="3">
+        <v>64358</v>
+      </c>
+      <c r="F195" s="3">
+        <v>46359</v>
+      </c>
+      <c r="G195" s="3">
+        <v>68268</v>
+      </c>
+      <c r="H195" s="3">
+        <v>45766</v>
+      </c>
+      <c r="I195" s="3">
+        <v>59969</v>
+      </c>
+      <c r="J195" s="3">
+        <v>39315</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>4</v>
       </c>
@@ -4697,10 +5493,28 @@
       </c>
       <c r="D196" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+        <v>322715</v>
+      </c>
+      <c r="E196" s="3">
+        <v>68670</v>
+      </c>
+      <c r="F196" s="3">
+        <v>41673</v>
+      </c>
+      <c r="G196" s="3">
+        <v>69065</v>
+      </c>
+      <c r="H196" s="3">
+        <v>40713</v>
+      </c>
+      <c r="I196" s="3">
+        <v>63612</v>
+      </c>
+      <c r="J196" s="3">
+        <v>38982</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>4</v>
       </c>
@@ -4712,10 +5526,28 @@
       </c>
       <c r="D197" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+        <v>333197</v>
+      </c>
+      <c r="E197" s="3">
+        <v>68540</v>
+      </c>
+      <c r="F197" s="3">
+        <v>44648</v>
+      </c>
+      <c r="G197" s="3">
+        <v>67333</v>
+      </c>
+      <c r="H197" s="3">
+        <v>46269</v>
+      </c>
+      <c r="I197" s="3">
+        <v>65772</v>
+      </c>
+      <c r="J197" s="3">
+        <v>40635</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>4</v>
       </c>
@@ -4727,10 +5559,28 @@
       </c>
       <c r="D198" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+        <v>319038</v>
+      </c>
+      <c r="E198" s="3">
+        <v>67864</v>
+      </c>
+      <c r="F198" s="3">
+        <v>40830</v>
+      </c>
+      <c r="G198" s="3">
+        <v>64809</v>
+      </c>
+      <c r="H198" s="3">
+        <v>42033</v>
+      </c>
+      <c r="I198" s="3">
+        <v>64312</v>
+      </c>
+      <c r="J198" s="3">
+        <v>39190</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>4</v>
       </c>
@@ -4742,10 +5592,28 @@
       </c>
       <c r="D199" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+        <v>321526</v>
+      </c>
+      <c r="E199" s="3">
+        <v>66823</v>
+      </c>
+      <c r="F199" s="3">
+        <v>39128</v>
+      </c>
+      <c r="G199" s="3">
+        <v>68160</v>
+      </c>
+      <c r="H199" s="3">
+        <v>45987</v>
+      </c>
+      <c r="I199" s="3">
+        <v>59536</v>
+      </c>
+      <c r="J199" s="3">
+        <v>41892</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>4</v>
       </c>
@@ -4757,10 +5625,28 @@
       </c>
       <c r="D200" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+        <v>339790</v>
+      </c>
+      <c r="E200" s="3">
+        <v>68486</v>
+      </c>
+      <c r="F200" s="3">
+        <v>45174</v>
+      </c>
+      <c r="G200" s="3">
+        <v>69417</v>
+      </c>
+      <c r="H200" s="3">
+        <v>45691</v>
+      </c>
+      <c r="I200" s="3">
+        <v>70035</v>
+      </c>
+      <c r="J200" s="3">
+        <v>40987</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>4</v>
       </c>
@@ -4772,10 +5658,28 @@
       </c>
       <c r="D201" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+        <v>344674</v>
+      </c>
+      <c r="E201" s="3">
+        <v>69871</v>
+      </c>
+      <c r="F201" s="3">
+        <v>46120</v>
+      </c>
+      <c r="G201" s="3">
+        <v>70882</v>
+      </c>
+      <c r="H201" s="3">
+        <v>43927</v>
+      </c>
+      <c r="I201" s="3">
+        <v>65975</v>
+      </c>
+      <c r="J201" s="3">
+        <v>47899</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>5</v>
       </c>
@@ -4787,10 +5691,13 @@
       </c>
       <c r="D202" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+        <v>163822</v>
+      </c>
+      <c r="E202" s="3">
+        <v>163822</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>5</v>
       </c>
@@ -4805,7 +5712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>5</v>
       </c>
@@ -4820,7 +5727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>5</v>
       </c>
@@ -4835,7 +5742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>5</v>
       </c>
@@ -4850,7 +5757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>5</v>
       </c>
@@ -4865,7 +5772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Add data for workflow 5 and 6
</commit_message>
<xml_diff>
--- a/workflow-analysis-and-rewrite/runtime-analysis-and-rewrite.xlsx
+++ b/workflow-analysis-and-rewrite/runtime-analysis-and-rewrite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wederbn\Desktop\Coding\PlanQK\qprov-content\workflow-analysis-and-rewrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EE2F30-3963-4F72-A19A-F6A7E464048D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9A18CE-7C85-450C-BEED-1C53C1C881D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{DFC69C5A-AAD8-407D-8907-336986DC4050}"/>
   </bookViews>
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4836293F-B9CB-4320-909E-74B95BB4C54A}">
   <dimension ref="A1:O351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C193" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,6 +669,10 @@
         <f>MEDIAN(C202:C251)</f>
         <v>398.5</v>
       </c>
+      <c r="O6">
+        <f>MEDIAN(D202:D251)</f>
+        <v>314537</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -697,6 +701,10 @@
         <f>MEDIAN(C252:C301)</f>
         <v>588</v>
       </c>
+      <c r="O7">
+        <f>MEDIAN(D252:D301)</f>
+        <v>631510.5</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -5691,10 +5699,13 @@
       </c>
       <c r="D202" s="3">
         <f t="shared" si="3"/>
-        <v>163822</v>
+        <v>322922</v>
       </c>
       <c r="E202" s="3">
         <v>163822</v>
+      </c>
+      <c r="F202" s="3">
+        <v>159100</v>
       </c>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.25">
@@ -5709,7 +5720,13 @@
       </c>
       <c r="D203" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>324231</v>
+      </c>
+      <c r="E203" s="3">
+        <v>159337</v>
+      </c>
+      <c r="F203" s="3">
+        <v>164894</v>
       </c>
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.25">
@@ -5724,7 +5741,13 @@
       </c>
       <c r="D204" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>319379</v>
+      </c>
+      <c r="E204" s="3">
+        <v>160551</v>
+      </c>
+      <c r="F204" s="3">
+        <v>158828</v>
       </c>
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.25">
@@ -5739,7 +5762,13 @@
       </c>
       <c r="D205" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>312270</v>
+      </c>
+      <c r="E205" s="3">
+        <v>158544</v>
+      </c>
+      <c r="F205" s="3">
+        <v>153726</v>
       </c>
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.25">
@@ -5754,7 +5783,13 @@
       </c>
       <c r="D206" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>313566</v>
+      </c>
+      <c r="E206" s="3">
+        <v>150363</v>
+      </c>
+      <c r="F206" s="3">
+        <v>163203</v>
       </c>
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.25">
@@ -5769,7 +5804,13 @@
       </c>
       <c r="D207" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>317845</v>
+      </c>
+      <c r="E207" s="3">
+        <v>165618</v>
+      </c>
+      <c r="F207" s="3">
+        <v>152227</v>
       </c>
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.25">
@@ -5784,10 +5825,16 @@
       </c>
       <c r="D208" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+        <v>324513</v>
+      </c>
+      <c r="E208" s="3">
+        <v>159523</v>
+      </c>
+      <c r="F208" s="3">
+        <v>164990</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>5</v>
       </c>
@@ -5799,10 +5846,16 @@
       </c>
       <c r="D209" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+        <v>313171</v>
+      </c>
+      <c r="E209" s="3">
+        <v>153556</v>
+      </c>
+      <c r="F209" s="3">
+        <v>159615</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>5</v>
       </c>
@@ -5814,10 +5867,16 @@
       </c>
       <c r="D210" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+        <v>315517</v>
+      </c>
+      <c r="E210" s="3">
+        <v>161040</v>
+      </c>
+      <c r="F210" s="3">
+        <v>154477</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>5</v>
       </c>
@@ -5829,10 +5888,16 @@
       </c>
       <c r="D211" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+        <v>313588</v>
+      </c>
+      <c r="E211" s="3">
+        <v>152403</v>
+      </c>
+      <c r="F211" s="3">
+        <v>161185</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>5</v>
       </c>
@@ -5844,10 +5909,16 @@
       </c>
       <c r="D212" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+        <v>306618</v>
+      </c>
+      <c r="E212" s="3">
+        <v>151619</v>
+      </c>
+      <c r="F212" s="3">
+        <v>154999</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>5</v>
       </c>
@@ -5859,10 +5930,16 @@
       </c>
       <c r="D213" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+        <v>303378</v>
+      </c>
+      <c r="E213" s="3">
+        <v>152868</v>
+      </c>
+      <c r="F213" s="3">
+        <v>150510</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>5</v>
       </c>
@@ -5874,10 +5951,16 @@
       </c>
       <c r="D214" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+        <v>314651</v>
+      </c>
+      <c r="E214" s="3">
+        <v>159477</v>
+      </c>
+      <c r="F214" s="3">
+        <v>155174</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>5</v>
       </c>
@@ -5889,10 +5972,16 @@
       </c>
       <c r="D215" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+        <v>313351</v>
+      </c>
+      <c r="E215" s="3">
+        <v>153661</v>
+      </c>
+      <c r="F215" s="3">
+        <v>159690</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>5</v>
       </c>
@@ -5904,10 +5993,16 @@
       </c>
       <c r="D216" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+        <v>315201</v>
+      </c>
+      <c r="E216" s="3">
+        <v>164736</v>
+      </c>
+      <c r="F216" s="3">
+        <v>150465</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>5</v>
       </c>
@@ -5919,10 +6014,16 @@
       </c>
       <c r="D217" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+        <v>311718</v>
+      </c>
+      <c r="E217" s="3">
+        <v>159666</v>
+      </c>
+      <c r="F217" s="3">
+        <v>152052</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>5</v>
       </c>
@@ -5934,10 +6035,16 @@
       </c>
       <c r="D218" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+        <v>305864</v>
+      </c>
+      <c r="E218" s="3">
+        <v>152611</v>
+      </c>
+      <c r="F218" s="3">
+        <v>153253</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>5</v>
       </c>
@@ -5949,10 +6056,16 @@
       </c>
       <c r="D219" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+        <v>305952</v>
+      </c>
+      <c r="E219" s="3">
+        <v>152710</v>
+      </c>
+      <c r="F219" s="3">
+        <v>153242</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>5</v>
       </c>
@@ -5964,10 +6077,16 @@
       </c>
       <c r="D220" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+        <v>314423</v>
+      </c>
+      <c r="E220" s="3">
+        <v>150112</v>
+      </c>
+      <c r="F220" s="3">
+        <v>164311</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>5</v>
       </c>
@@ -5979,10 +6098,16 @@
       </c>
       <c r="D221" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+        <v>313709</v>
+      </c>
+      <c r="E221" s="3">
+        <v>156454</v>
+      </c>
+      <c r="F221" s="3">
+        <v>157255</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>5</v>
       </c>
@@ -5994,10 +6119,16 @@
       </c>
       <c r="D222" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+        <v>307538</v>
+      </c>
+      <c r="E222" s="3">
+        <v>156561</v>
+      </c>
+      <c r="F222" s="3">
+        <v>150977</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>5</v>
       </c>
@@ -6009,10 +6140,16 @@
       </c>
       <c r="D223" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+        <v>315577</v>
+      </c>
+      <c r="E223" s="3">
+        <v>155807</v>
+      </c>
+      <c r="F223" s="3">
+        <v>159770</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>5</v>
       </c>
@@ -6024,10 +6161,16 @@
       </c>
       <c r="D224" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+        <v>323216</v>
+      </c>
+      <c r="E224" s="3">
+        <v>159556</v>
+      </c>
+      <c r="F224" s="3">
+        <v>163660</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>5</v>
       </c>
@@ -6039,10 +6182,16 @@
       </c>
       <c r="D225" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+        <v>311817</v>
+      </c>
+      <c r="E225" s="3">
+        <v>156591</v>
+      </c>
+      <c r="F225" s="3">
+        <v>155226</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>5</v>
       </c>
@@ -6054,10 +6203,16 @@
       </c>
       <c r="D226" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+        <v>316969</v>
+      </c>
+      <c r="E226" s="3">
+        <v>159147</v>
+      </c>
+      <c r="F226" s="3">
+        <v>157822</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>5</v>
       </c>
@@ -6069,10 +6224,16 @@
       </c>
       <c r="D227" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+        <v>319491</v>
+      </c>
+      <c r="E227" s="3">
+        <v>155404</v>
+      </c>
+      <c r="F227" s="3">
+        <v>164087</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>5</v>
       </c>
@@ -6084,10 +6245,16 @@
       </c>
       <c r="D228" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+        <v>320980</v>
+      </c>
+      <c r="E228" s="3">
+        <v>160072</v>
+      </c>
+      <c r="F228" s="3">
+        <v>160908</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>5</v>
       </c>
@@ -6099,10 +6266,16 @@
       </c>
       <c r="D229" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+        <v>313239</v>
+      </c>
+      <c r="E229" s="3">
+        <v>153562</v>
+      </c>
+      <c r="F229" s="3">
+        <v>159677</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>5</v>
       </c>
@@ -6114,10 +6287,16 @@
       </c>
       <c r="D230" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+        <v>319404</v>
+      </c>
+      <c r="E230" s="3">
+        <v>161480</v>
+      </c>
+      <c r="F230" s="3">
+        <v>157924</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>5</v>
       </c>
@@ -6129,10 +6308,16 @@
       </c>
       <c r="D231" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+        <v>313189</v>
+      </c>
+      <c r="E231" s="3">
+        <v>153238</v>
+      </c>
+      <c r="F231" s="3">
+        <v>159951</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>5</v>
       </c>
@@ -6144,10 +6329,16 @@
       </c>
       <c r="D232" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+        <v>317064</v>
+      </c>
+      <c r="E232" s="3">
+        <v>154199</v>
+      </c>
+      <c r="F232" s="3">
+        <v>162865</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>5</v>
       </c>
@@ -6159,10 +6350,16 @@
       </c>
       <c r="D233" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+        <v>308683</v>
+      </c>
+      <c r="E233" s="3">
+        <v>152944</v>
+      </c>
+      <c r="F233" s="3">
+        <v>155739</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>5</v>
       </c>
@@ -6174,10 +6371,16 @@
       </c>
       <c r="D234" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+        <v>320938</v>
+      </c>
+      <c r="E234" s="3">
+        <v>158899</v>
+      </c>
+      <c r="F234" s="3">
+        <v>162039</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>5</v>
       </c>
@@ -6189,10 +6392,16 @@
       </c>
       <c r="D235" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+        <v>323609</v>
+      </c>
+      <c r="E235" s="3">
+        <v>158597</v>
+      </c>
+      <c r="F235" s="3">
+        <v>165012</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>5</v>
       </c>
@@ -6204,10 +6413,16 @@
       </c>
       <c r="D236" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+        <v>305078</v>
+      </c>
+      <c r="E236" s="3">
+        <v>151128</v>
+      </c>
+      <c r="F236" s="3">
+        <v>153950</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>5</v>
       </c>
@@ -6219,10 +6434,16 @@
       </c>
       <c r="D237" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+        <v>310771</v>
+      </c>
+      <c r="E237" s="3">
+        <v>152578</v>
+      </c>
+      <c r="F237" s="3">
+        <v>158193</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>5</v>
       </c>
@@ -6234,10 +6455,16 @@
       </c>
       <c r="D238" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+        <v>305763</v>
+      </c>
+      <c r="E238" s="3">
+        <v>151674</v>
+      </c>
+      <c r="F238" s="3">
+        <v>154089</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>5</v>
       </c>
@@ -6249,10 +6476,16 @@
       </c>
       <c r="D239" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+        <v>310825</v>
+      </c>
+      <c r="E239" s="3">
+        <v>155734</v>
+      </c>
+      <c r="F239" s="3">
+        <v>155091</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>5</v>
       </c>
@@ -6264,10 +6497,16 @@
       </c>
       <c r="D240" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+        <v>327327</v>
+      </c>
+      <c r="E240" s="3">
+        <v>162852</v>
+      </c>
+      <c r="F240" s="3">
+        <v>164475</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>5</v>
       </c>
@@ -6279,10 +6518,16 @@
       </c>
       <c r="D241" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+        <v>317224</v>
+      </c>
+      <c r="E241" s="3">
+        <v>158737</v>
+      </c>
+      <c r="F241" s="3">
+        <v>158487</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>5</v>
       </c>
@@ -6294,10 +6539,16 @@
       </c>
       <c r="D242" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+        <v>315172</v>
+      </c>
+      <c r="E242" s="3">
+        <v>157942</v>
+      </c>
+      <c r="F242" s="3">
+        <v>157230</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>5</v>
       </c>
@@ -6309,10 +6560,16 @@
       </c>
       <c r="D243" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+        <v>308988</v>
+      </c>
+      <c r="E243" s="3">
+        <v>151141</v>
+      </c>
+      <c r="F243" s="3">
+        <v>157847</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>5</v>
       </c>
@@ -6324,10 +6581,16 @@
       </c>
       <c r="D244" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+        <v>319999</v>
+      </c>
+      <c r="E244" s="3">
+        <v>161896</v>
+      </c>
+      <c r="F244" s="3">
+        <v>158103</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>5</v>
       </c>
@@ -6339,10 +6602,16 @@
       </c>
       <c r="D245" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+        <v>307851</v>
+      </c>
+      <c r="E245" s="3">
+        <v>155834</v>
+      </c>
+      <c r="F245" s="3">
+        <v>152017</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>5</v>
       </c>
@@ -6354,10 +6623,16 @@
       </c>
       <c r="D246" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+        <v>313700</v>
+      </c>
+      <c r="E246" s="3">
+        <v>157392</v>
+      </c>
+      <c r="F246" s="3">
+        <v>156308</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>5</v>
       </c>
@@ -6369,10 +6644,16 @@
       </c>
       <c r="D247" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+        <v>328760</v>
+      </c>
+      <c r="E247" s="3">
+        <v>165203</v>
+      </c>
+      <c r="F247" s="3">
+        <v>163557</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>5</v>
       </c>
@@ -6384,10 +6665,16 @@
       </c>
       <c r="D248" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+        <v>309270</v>
+      </c>
+      <c r="E248" s="3">
+        <v>154347</v>
+      </c>
+      <c r="F248" s="3">
+        <v>154923</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>5</v>
       </c>
@@ -6399,10 +6686,16 @@
       </c>
       <c r="D249" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+        <v>322063</v>
+      </c>
+      <c r="E249" s="3">
+        <v>161844</v>
+      </c>
+      <c r="F249" s="3">
+        <v>160219</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>5</v>
       </c>
@@ -6414,10 +6707,16 @@
       </c>
       <c r="D250" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+        <v>320434</v>
+      </c>
+      <c r="E250" s="3">
+        <v>155318</v>
+      </c>
+      <c r="F250" s="3">
+        <v>165116</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>5</v>
       </c>
@@ -6429,10 +6728,16 @@
       </c>
       <c r="D251" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+        <v>316122</v>
+      </c>
+      <c r="E251" s="3">
+        <v>165821</v>
+      </c>
+      <c r="F251" s="3">
+        <v>150301</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>6</v>
       </c>
@@ -6444,10 +6749,22 @@
       </c>
       <c r="D252" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+        <v>621756</v>
+      </c>
+      <c r="E252" s="3">
+        <v>163768</v>
+      </c>
+      <c r="F252" s="3">
+        <v>156248</v>
+      </c>
+      <c r="G252" s="3">
+        <v>150805</v>
+      </c>
+      <c r="H252" s="3">
+        <v>150935</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>6</v>
       </c>
@@ -6459,10 +6776,22 @@
       </c>
       <c r="D253" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+        <v>615117</v>
+      </c>
+      <c r="E253" s="3">
+        <v>156798</v>
+      </c>
+      <c r="F253" s="3">
+        <v>151865</v>
+      </c>
+      <c r="G253" s="3">
+        <v>155129</v>
+      </c>
+      <c r="H253" s="3">
+        <v>151325</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>6</v>
       </c>
@@ -6474,10 +6803,22 @@
       </c>
       <c r="D254" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+        <v>633775</v>
+      </c>
+      <c r="E254" s="3">
+        <v>152377</v>
+      </c>
+      <c r="F254" s="3">
+        <v>155488</v>
+      </c>
+      <c r="G254" s="3">
+        <v>162814</v>
+      </c>
+      <c r="H254" s="3">
+        <v>163096</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>6</v>
       </c>
@@ -6489,10 +6830,22 @@
       </c>
       <c r="D255" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+        <v>648139</v>
+      </c>
+      <c r="E255" s="3">
+        <v>160436</v>
+      </c>
+      <c r="F255" s="3">
+        <v>163693</v>
+      </c>
+      <c r="G255" s="4">
+        <v>160166</v>
+      </c>
+      <c r="H255" s="3">
+        <v>163844</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>6</v>
       </c>
@@ -6504,10 +6857,22 @@
       </c>
       <c r="D256" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+        <v>634364</v>
+      </c>
+      <c r="E256" s="3">
+        <v>154043</v>
+      </c>
+      <c r="F256" s="3">
+        <v>163932</v>
+      </c>
+      <c r="G256" s="3">
+        <v>152181</v>
+      </c>
+      <c r="H256" s="3">
+        <v>164208</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>6</v>
       </c>
@@ -6519,10 +6884,22 @@
       </c>
       <c r="D257" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+        <v>627815</v>
+      </c>
+      <c r="E257" s="3">
+        <v>154497</v>
+      </c>
+      <c r="F257" s="3">
+        <v>157050</v>
+      </c>
+      <c r="G257" s="3">
+        <v>162121</v>
+      </c>
+      <c r="H257" s="3">
+        <v>154147</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>6</v>
       </c>
@@ -6534,10 +6911,22 @@
       </c>
       <c r="D258" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+        <v>635847</v>
+      </c>
+      <c r="E258" s="3">
+        <v>154958</v>
+      </c>
+      <c r="F258" s="3">
+        <v>157406</v>
+      </c>
+      <c r="G258" s="3">
+        <v>161509</v>
+      </c>
+      <c r="H258" s="3">
+        <v>161974</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>6</v>
       </c>
@@ -6549,10 +6938,22 @@
       </c>
       <c r="D259" s="3">
         <f t="shared" ref="D259:D322" si="4">SUM(E259:J259)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+        <v>641197</v>
+      </c>
+      <c r="E259" s="3">
+        <v>162234</v>
+      </c>
+      <c r="F259" s="3">
+        <v>158161</v>
+      </c>
+      <c r="G259" s="3">
+        <v>156287</v>
+      </c>
+      <c r="H259" s="3">
+        <v>164515</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>6</v>
       </c>
@@ -6564,10 +6965,22 @@
       </c>
       <c r="D260" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+        <v>631267</v>
+      </c>
+      <c r="E260" s="3">
+        <v>153233</v>
+      </c>
+      <c r="F260" s="3">
+        <v>163724</v>
+      </c>
+      <c r="G260" s="3">
+        <v>162823</v>
+      </c>
+      <c r="H260" s="3">
+        <v>151487</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>6</v>
       </c>
@@ -6579,10 +6992,22 @@
       </c>
       <c r="D261" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+        <v>637725</v>
+      </c>
+      <c r="E261" s="3">
+        <v>158818</v>
+      </c>
+      <c r="F261" s="3">
+        <v>156830</v>
+      </c>
+      <c r="G261" s="3">
+        <v>163008</v>
+      </c>
+      <c r="H261" s="3">
+        <v>159069</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>6</v>
       </c>
@@ -6594,10 +7019,22 @@
       </c>
       <c r="D262" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+        <v>625359</v>
+      </c>
+      <c r="E262" s="3">
+        <v>150679</v>
+      </c>
+      <c r="F262" s="3">
+        <v>160348</v>
+      </c>
+      <c r="G262" s="3">
+        <v>162938</v>
+      </c>
+      <c r="H262" s="3">
+        <v>151394</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>6</v>
       </c>
@@ -6609,10 +7046,22 @@
       </c>
       <c r="D263" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+        <v>642048</v>
+      </c>
+      <c r="E263" s="3">
+        <v>162222</v>
+      </c>
+      <c r="F263" s="3">
+        <v>164608</v>
+      </c>
+      <c r="G263" s="3">
+        <v>153818</v>
+      </c>
+      <c r="H263" s="3">
+        <v>161400</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>6</v>
       </c>
@@ -6624,10 +7073,22 @@
       </c>
       <c r="D264" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+        <v>626542</v>
+      </c>
+      <c r="E264" s="3">
+        <v>162621</v>
+      </c>
+      <c r="F264" s="3">
+        <v>154587</v>
+      </c>
+      <c r="G264" s="3">
+        <v>150666</v>
+      </c>
+      <c r="H264" s="3">
+        <v>158668</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>6</v>
       </c>
@@ -6639,10 +7100,22 @@
       </c>
       <c r="D265" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+        <v>614321</v>
+      </c>
+      <c r="E265" s="3">
+        <v>150606</v>
+      </c>
+      <c r="F265" s="3">
+        <v>154604</v>
+      </c>
+      <c r="G265" s="3">
+        <v>157360</v>
+      </c>
+      <c r="H265" s="3">
+        <v>151751</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>6</v>
       </c>
@@ -6654,10 +7127,22 @@
       </c>
       <c r="D266" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+        <v>617345</v>
+      </c>
+      <c r="E266" s="3">
+        <v>164397</v>
+      </c>
+      <c r="F266" s="3">
+        <v>150072</v>
+      </c>
+      <c r="G266" s="3">
+        <v>151025</v>
+      </c>
+      <c r="H266" s="3">
+        <v>151851</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>6</v>
       </c>
@@ -6669,10 +7154,22 @@
       </c>
       <c r="D267" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+        <v>624362</v>
+      </c>
+      <c r="E267" s="3">
+        <v>162936</v>
+      </c>
+      <c r="F267" s="3">
+        <v>157198</v>
+      </c>
+      <c r="G267" s="3">
+        <v>153115</v>
+      </c>
+      <c r="H267" s="3">
+        <v>151113</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>6</v>
       </c>
@@ -6684,10 +7181,22 @@
       </c>
       <c r="D268" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+        <v>643451</v>
+      </c>
+      <c r="E268" s="3">
+        <v>151023</v>
+      </c>
+      <c r="F268" s="3">
+        <v>162964</v>
+      </c>
+      <c r="G268" s="3">
+        <v>164969</v>
+      </c>
+      <c r="H268" s="3">
+        <v>164495</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>6</v>
       </c>
@@ -6699,10 +7208,22 @@
       </c>
       <c r="D269" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+        <v>628940</v>
+      </c>
+      <c r="E269" s="3">
+        <v>157233</v>
+      </c>
+      <c r="F269" s="3">
+        <v>156577</v>
+      </c>
+      <c r="G269" s="3">
+        <v>150629</v>
+      </c>
+      <c r="H269" s="3">
+        <v>164501</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>6</v>
       </c>
@@ -6714,10 +7235,22 @@
       </c>
       <c r="D270" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+        <v>627664</v>
+      </c>
+      <c r="E270" s="3">
+        <v>162545</v>
+      </c>
+      <c r="F270" s="3">
+        <v>157236</v>
+      </c>
+      <c r="G270" s="3">
+        <v>156917</v>
+      </c>
+      <c r="H270" s="3">
+        <v>150966</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>6</v>
       </c>
@@ -6729,10 +7262,22 @@
       </c>
       <c r="D271" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+        <v>630919</v>
+      </c>
+      <c r="E271" s="3">
+        <v>156954</v>
+      </c>
+      <c r="F271" s="3">
+        <v>159831</v>
+      </c>
+      <c r="G271" s="3">
+        <v>156138</v>
+      </c>
+      <c r="H271" s="3">
+        <v>157996</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>6</v>
       </c>
@@ -6744,10 +7289,22 @@
       </c>
       <c r="D272" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+        <v>633969</v>
+      </c>
+      <c r="E272" s="3">
+        <v>151906</v>
+      </c>
+      <c r="F272" s="3">
+        <v>152253</v>
+      </c>
+      <c r="G272" s="3">
+        <v>164961</v>
+      </c>
+      <c r="H272" s="3">
+        <v>164849</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>6</v>
       </c>
@@ -6759,10 +7316,22 @@
       </c>
       <c r="D273" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+        <v>637026</v>
+      </c>
+      <c r="E273" s="3">
+        <v>164286</v>
+      </c>
+      <c r="F273" s="3">
+        <v>157173</v>
+      </c>
+      <c r="G273" s="3">
+        <v>160603</v>
+      </c>
+      <c r="H273" s="3">
+        <v>154964</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>6</v>
       </c>
@@ -6774,10 +7343,22 @@
       </c>
       <c r="D274" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+        <v>628980</v>
+      </c>
+      <c r="E274" s="3">
+        <v>162120</v>
+      </c>
+      <c r="F274" s="3">
+        <v>155517</v>
+      </c>
+      <c r="G274" s="3">
+        <v>155794</v>
+      </c>
+      <c r="H274" s="3">
+        <v>155549</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>6</v>
       </c>
@@ -6789,10 +7370,22 @@
       </c>
       <c r="D275" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+        <v>649429</v>
+      </c>
+      <c r="E275" s="3">
+        <v>161575</v>
+      </c>
+      <c r="F275" s="3">
+        <v>162239</v>
+      </c>
+      <c r="G275" s="3">
+        <v>162604</v>
+      </c>
+      <c r="H275" s="3">
+        <v>163011</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>6</v>
       </c>
@@ -6804,10 +7397,22 @@
       </c>
       <c r="D276" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+        <v>646520</v>
+      </c>
+      <c r="E276" s="3">
+        <v>164308</v>
+      </c>
+      <c r="F276" s="3">
+        <v>161760</v>
+      </c>
+      <c r="G276" s="3">
+        <v>163021</v>
+      </c>
+      <c r="H276" s="3">
+        <v>157431</v>
+      </c>
+    </row>
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>6</v>
       </c>
@@ -6819,10 +7424,22 @@
       </c>
       <c r="D277" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+        <v>640933</v>
+      </c>
+      <c r="E277" s="3">
+        <v>154911</v>
+      </c>
+      <c r="F277" s="3">
+        <v>161205</v>
+      </c>
+      <c r="G277" s="3">
+        <v>164086</v>
+      </c>
+      <c r="H277" s="3">
+        <v>160731</v>
+      </c>
+    </row>
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>6</v>
       </c>
@@ -6834,10 +7451,22 @@
       </c>
       <c r="D278" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+        <v>637687</v>
+      </c>
+      <c r="E278" s="3">
+        <v>164221</v>
+      </c>
+      <c r="F278" s="3">
+        <v>153163</v>
+      </c>
+      <c r="G278" s="3">
+        <v>157152</v>
+      </c>
+      <c r="H278" s="3">
+        <v>163151</v>
+      </c>
+    </row>
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>6</v>
       </c>
@@ -6849,10 +7478,22 @@
       </c>
       <c r="D279" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+        <v>648325</v>
+      </c>
+      <c r="E279" s="3">
+        <v>164338</v>
+      </c>
+      <c r="F279" s="3">
+        <v>164326</v>
+      </c>
+      <c r="G279" s="3">
+        <v>160598</v>
+      </c>
+      <c r="H279" s="3">
+        <v>159063</v>
+      </c>
+    </row>
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>6</v>
       </c>
@@ -6864,10 +7505,22 @@
       </c>
       <c r="D280" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+        <v>617409</v>
+      </c>
+      <c r="E280" s="3">
+        <v>151328</v>
+      </c>
+      <c r="F280" s="3">
+        <v>154259</v>
+      </c>
+      <c r="G280" s="3">
+        <v>152006</v>
+      </c>
+      <c r="H280" s="3">
+        <v>159816</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>6</v>
       </c>
@@ -6879,10 +7532,22 @@
       </c>
       <c r="D281" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+        <v>633811</v>
+      </c>
+      <c r="E281" s="3">
+        <v>162944</v>
+      </c>
+      <c r="F281" s="3">
+        <v>152255</v>
+      </c>
+      <c r="G281" s="3">
+        <v>156600</v>
+      </c>
+      <c r="H281" s="3">
+        <v>162012</v>
+      </c>
+    </row>
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>6</v>
       </c>
@@ -6894,10 +7559,22 @@
       </c>
       <c r="D282" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+        <v>627991</v>
+      </c>
+      <c r="E282" s="3">
+        <v>161759</v>
+      </c>
+      <c r="F282" s="3">
+        <v>150395</v>
+      </c>
+      <c r="G282" s="3">
+        <v>162612</v>
+      </c>
+      <c r="H282" s="3">
+        <v>153225</v>
+      </c>
+    </row>
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>6</v>
       </c>
@@ -6909,10 +7586,22 @@
       </c>
       <c r="D283" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+        <v>643855</v>
+      </c>
+      <c r="E283" s="3">
+        <v>161335</v>
+      </c>
+      <c r="F283" s="3">
+        <v>156555</v>
+      </c>
+      <c r="G283" s="3">
+        <v>161931</v>
+      </c>
+      <c r="H283" s="3">
+        <v>164034</v>
+      </c>
+    </row>
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>6</v>
       </c>
@@ -6924,10 +7613,22 @@
       </c>
       <c r="D284" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+        <v>631975</v>
+      </c>
+      <c r="E284" s="3">
+        <v>159011</v>
+      </c>
+      <c r="F284" s="3">
+        <v>157497</v>
+      </c>
+      <c r="G284" s="3">
+        <v>163623</v>
+      </c>
+      <c r="H284" s="3">
+        <v>151844</v>
+      </c>
+    </row>
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>6</v>
       </c>
@@ -6939,10 +7640,22 @@
       </c>
       <c r="D285" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+        <v>629068</v>
+      </c>
+      <c r="E285" s="3">
+        <v>161671</v>
+      </c>
+      <c r="F285" s="3">
+        <v>156104</v>
+      </c>
+      <c r="G285" s="3">
+        <v>159550</v>
+      </c>
+      <c r="H285" s="3">
+        <v>151743</v>
+      </c>
+    </row>
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>6</v>
       </c>
@@ -6954,10 +7667,22 @@
       </c>
       <c r="D286" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+        <v>633650</v>
+      </c>
+      <c r="E286" s="3">
+        <v>157437</v>
+      </c>
+      <c r="F286" s="3">
+        <v>150679</v>
+      </c>
+      <c r="G286" s="3">
+        <v>162162</v>
+      </c>
+      <c r="H286" s="3">
+        <v>163372</v>
+      </c>
+    </row>
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>6</v>
       </c>
@@ -6969,10 +7694,22 @@
       </c>
       <c r="D287" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+        <v>625533</v>
+      </c>
+      <c r="E287" s="3">
+        <v>150531</v>
+      </c>
+      <c r="F287" s="3">
+        <v>161798</v>
+      </c>
+      <c r="G287" s="3">
+        <v>152074</v>
+      </c>
+      <c r="H287" s="3">
+        <v>161130</v>
+      </c>
+    </row>
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>6</v>
       </c>
@@ -6984,10 +7721,22 @@
       </c>
       <c r="D288" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+        <v>624776</v>
+      </c>
+      <c r="E288" s="3">
+        <v>150259</v>
+      </c>
+      <c r="F288" s="3">
+        <v>159741</v>
+      </c>
+      <c r="G288" s="3">
+        <v>157966</v>
+      </c>
+      <c r="H288" s="3">
+        <v>156810</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>6</v>
       </c>
@@ -6999,10 +7748,22 @@
       </c>
       <c r="D289" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+        <v>616087</v>
+      </c>
+      <c r="E289" s="3">
+        <v>156301</v>
+      </c>
+      <c r="F289" s="3">
+        <v>158152</v>
+      </c>
+      <c r="G289" s="3">
+        <v>150850</v>
+      </c>
+      <c r="H289" s="3">
+        <v>150784</v>
+      </c>
+    </row>
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>6</v>
       </c>
@@ -7014,10 +7775,22 @@
       </c>
       <c r="D290" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+        <v>625183</v>
+      </c>
+      <c r="E290" s="3">
+        <v>157562</v>
+      </c>
+      <c r="F290" s="3">
+        <v>157133</v>
+      </c>
+      <c r="G290" s="3">
+        <v>153233</v>
+      </c>
+      <c r="H290" s="3">
+        <v>157255</v>
+      </c>
+    </row>
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>6</v>
       </c>
@@ -7029,10 +7802,22 @@
       </c>
       <c r="D291" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+        <v>631114</v>
+      </c>
+      <c r="E291" s="3">
+        <v>156278</v>
+      </c>
+      <c r="F291" s="3">
+        <v>160996</v>
+      </c>
+      <c r="G291" s="3">
+        <v>158626</v>
+      </c>
+      <c r="H291" s="3">
+        <v>155214</v>
+      </c>
+    </row>
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>6</v>
       </c>
@@ -7044,10 +7829,22 @@
       </c>
       <c r="D292" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+        <v>640110</v>
+      </c>
+      <c r="E292" s="3">
+        <v>153347</v>
+      </c>
+      <c r="F292" s="3">
+        <v>161870</v>
+      </c>
+      <c r="G292" s="3">
+        <v>160442</v>
+      </c>
+      <c r="H292" s="3">
+        <v>164451</v>
+      </c>
+    </row>
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>6</v>
       </c>
@@ -7059,10 +7856,22 @@
       </c>
       <c r="D293" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+        <v>648607</v>
+      </c>
+      <c r="E293" s="3">
+        <v>158524</v>
+      </c>
+      <c r="F293" s="3">
+        <v>162992</v>
+      </c>
+      <c r="G293" s="3">
+        <v>163224</v>
+      </c>
+      <c r="H293" s="3">
+        <v>163867</v>
+      </c>
+    </row>
+    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>6</v>
       </c>
@@ -7074,10 +7883,22 @@
       </c>
       <c r="D294" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+        <v>623306</v>
+      </c>
+      <c r="E294" s="3">
+        <v>159209</v>
+      </c>
+      <c r="F294" s="3">
+        <v>158482</v>
+      </c>
+      <c r="G294" s="3">
+        <v>153842</v>
+      </c>
+      <c r="H294" s="3">
+        <v>151773</v>
+      </c>
+    </row>
+    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>6</v>
       </c>
@@ -7089,10 +7910,22 @@
       </c>
       <c r="D295" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+        <v>633179</v>
+      </c>
+      <c r="E295" s="3">
+        <v>157325</v>
+      </c>
+      <c r="F295" s="3">
+        <v>152806</v>
+      </c>
+      <c r="G295" s="3">
+        <v>162303</v>
+      </c>
+      <c r="H295" s="3">
+        <v>160745</v>
+      </c>
+    </row>
+    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>6</v>
       </c>
@@ -7104,10 +7937,22 @@
       </c>
       <c r="D296" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+        <v>631659</v>
+      </c>
+      <c r="E296" s="3">
+        <v>157180</v>
+      </c>
+      <c r="F296" s="3">
+        <v>156799</v>
+      </c>
+      <c r="G296" s="3">
+        <v>152813</v>
+      </c>
+      <c r="H296" s="3">
+        <v>164867</v>
+      </c>
+    </row>
+    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>6</v>
       </c>
@@ -7119,10 +7964,22 @@
       </c>
       <c r="D297" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+        <v>618891</v>
+      </c>
+      <c r="E297" s="3">
+        <v>152912</v>
+      </c>
+      <c r="F297" s="3">
+        <v>154367</v>
+      </c>
+      <c r="G297" s="3">
+        <v>157520</v>
+      </c>
+      <c r="H297" s="3">
+        <v>154092</v>
+      </c>
+    </row>
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>6</v>
       </c>
@@ -7134,10 +7991,22 @@
       </c>
       <c r="D298" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+        <v>628171</v>
+      </c>
+      <c r="E298" s="3">
+        <v>161601</v>
+      </c>
+      <c r="F298" s="3">
+        <v>152574</v>
+      </c>
+      <c r="G298" s="3">
+        <v>153338</v>
+      </c>
+      <c r="H298" s="3">
+        <v>160658</v>
+      </c>
+    </row>
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>6</v>
       </c>
@@ -7149,10 +8018,22 @@
       </c>
       <c r="D299" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+        <v>642185</v>
+      </c>
+      <c r="E299" s="3">
+        <v>155434</v>
+      </c>
+      <c r="F299" s="3">
+        <v>163578</v>
+      </c>
+      <c r="G299" s="3">
+        <v>159628</v>
+      </c>
+      <c r="H299" s="3">
+        <v>163545</v>
+      </c>
+    </row>
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>6</v>
       </c>
@@ -7164,10 +8045,22 @@
       </c>
       <c r="D300" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+        <v>631362</v>
+      </c>
+      <c r="E300" s="3">
+        <v>159306</v>
+      </c>
+      <c r="F300" s="3">
+        <v>155327</v>
+      </c>
+      <c r="G300" s="3">
+        <v>161370</v>
+      </c>
+      <c r="H300" s="3">
+        <v>155359</v>
+      </c>
+    </row>
+    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>6</v>
       </c>
@@ -7179,10 +8072,22 @@
       </c>
       <c r="D301" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+        <v>635904</v>
+      </c>
+      <c r="E301" s="3">
+        <v>164305</v>
+      </c>
+      <c r="F301" s="3">
+        <v>157866</v>
+      </c>
+      <c r="G301" s="3">
+        <v>157323</v>
+      </c>
+      <c r="H301" s="3">
+        <v>156410</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>7</v>
       </c>
@@ -7197,7 +8102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>7</v>
       </c>
@@ -7212,7 +8117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Add first 25 runes for workflow 7
</commit_message>
<xml_diff>
--- a/workflow-analysis-and-rewrite/runtime-analysis-and-rewrite.xlsx
+++ b/workflow-analysis-and-rewrite/runtime-analysis-and-rewrite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wederbn\Desktop\Coding\PlanQK\qprov-content\workflow-analysis-and-rewrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9A18CE-7C85-450C-BEED-1C53C1C881D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B363ABA-FD63-40D3-A200-ED1776607D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{DFC69C5A-AAD8-407D-8907-336986DC4050}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{DFC69C5A-AAD8-407D-8907-336986DC4050}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4836293F-B9CB-4320-909E-74B95BB4C54A}">
   <dimension ref="A1:O351"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="A313" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,6 +733,10 @@
         <f>MEDIAN(C302:C351)</f>
         <v>733</v>
       </c>
+      <c r="O8">
+        <f>MEDIAN(D302:D351)</f>
+        <v>457355</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -7736,7 +7740,7 @@
         <v>156810</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>6</v>
       </c>
@@ -7763,7 +7767,7 @@
         <v>150784</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>6</v>
       </c>
@@ -7790,7 +7794,7 @@
         <v>157255</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>6</v>
       </c>
@@ -7817,7 +7821,7 @@
         <v>155214</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>6</v>
       </c>
@@ -7844,7 +7848,7 @@
         <v>164451</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>6</v>
       </c>
@@ -7871,7 +7875,7 @@
         <v>163867</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>6</v>
       </c>
@@ -7898,7 +7902,7 @@
         <v>151773</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>6</v>
       </c>
@@ -7925,7 +7929,7 @@
         <v>160745</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>6</v>
       </c>
@@ -7952,7 +7956,7 @@
         <v>164867</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>6</v>
       </c>
@@ -7979,7 +7983,7 @@
         <v>154092</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>6</v>
       </c>
@@ -8006,7 +8010,7 @@
         <v>160658</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>6</v>
       </c>
@@ -8033,7 +8037,7 @@
         <v>163545</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>6</v>
       </c>
@@ -8060,7 +8064,7 @@
         <v>155359</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>6</v>
       </c>
@@ -8087,7 +8091,7 @@
         <v>156410</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>7</v>
       </c>
@@ -8099,10 +8103,28 @@
       </c>
       <c r="D302" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+        <v>948715</v>
+      </c>
+      <c r="E302" s="3">
+        <v>158574</v>
+      </c>
+      <c r="F302" s="3">
+        <v>160663</v>
+      </c>
+      <c r="G302" s="3">
+        <v>163370</v>
+      </c>
+      <c r="H302" s="3">
+        <v>161046</v>
+      </c>
+      <c r="I302" s="3">
+        <v>154067</v>
+      </c>
+      <c r="J302" s="3">
+        <v>150995</v>
+      </c>
+    </row>
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>7</v>
       </c>
@@ -8114,10 +8136,28 @@
       </c>
       <c r="D303" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
+        <v>934665</v>
+      </c>
+      <c r="E303" s="3">
+        <v>161658</v>
+      </c>
+      <c r="F303" s="3">
+        <v>157946</v>
+      </c>
+      <c r="G303" s="3">
+        <v>157214</v>
+      </c>
+      <c r="H303" s="3">
+        <v>157868</v>
+      </c>
+      <c r="I303" s="3">
+        <v>151516</v>
+      </c>
+      <c r="J303" s="3">
+        <v>148463</v>
+      </c>
+    </row>
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>7</v>
       </c>
@@ -8129,10 +8169,28 @@
       </c>
       <c r="D304" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+        <v>919141</v>
+      </c>
+      <c r="E304" s="3">
+        <v>149064</v>
+      </c>
+      <c r="F304" s="3">
+        <v>153583</v>
+      </c>
+      <c r="G304" s="3">
+        <v>151478</v>
+      </c>
+      <c r="H304" s="3">
+        <v>160312</v>
+      </c>
+      <c r="I304" s="3">
+        <v>148263</v>
+      </c>
+      <c r="J304" s="3">
+        <v>156441</v>
+      </c>
+    </row>
+    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>7</v>
       </c>
@@ -8144,10 +8202,28 @@
       </c>
       <c r="D305" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+        <v>937339</v>
+      </c>
+      <c r="E305" s="3">
+        <v>151316</v>
+      </c>
+      <c r="F305" s="3">
+        <v>157481</v>
+      </c>
+      <c r="G305" s="3">
+        <v>155128</v>
+      </c>
+      <c r="H305" s="3">
+        <v>162789</v>
+      </c>
+      <c r="I305" s="3">
+        <v>161158</v>
+      </c>
+      <c r="J305" s="3">
+        <v>149467</v>
+      </c>
+    </row>
+    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>7</v>
       </c>
@@ -8159,10 +8235,28 @@
       </c>
       <c r="D306" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+        <v>945225</v>
+      </c>
+      <c r="E306" s="3">
+        <v>160669</v>
+      </c>
+      <c r="F306" s="3">
+        <v>155505</v>
+      </c>
+      <c r="G306" s="3">
+        <v>161425</v>
+      </c>
+      <c r="H306" s="3">
+        <v>151684</v>
+      </c>
+      <c r="I306" s="3">
+        <v>159768</v>
+      </c>
+      <c r="J306" s="3">
+        <v>156174</v>
+      </c>
+    </row>
+    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>7</v>
       </c>
@@ -8174,10 +8268,28 @@
       </c>
       <c r="D307" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+        <v>928403</v>
+      </c>
+      <c r="E307" s="3">
+        <v>149744</v>
+      </c>
+      <c r="F307" s="3">
+        <v>160431</v>
+      </c>
+      <c r="G307" s="3">
+        <v>149443</v>
+      </c>
+      <c r="H307" s="3">
+        <v>154114</v>
+      </c>
+      <c r="I307" s="3">
+        <v>153019</v>
+      </c>
+      <c r="J307" s="3">
+        <v>161652</v>
+      </c>
+    </row>
+    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>7</v>
       </c>
@@ -8189,10 +8301,28 @@
       </c>
       <c r="D308" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+        <v>932226</v>
+      </c>
+      <c r="E308" s="3">
+        <v>148234</v>
+      </c>
+      <c r="F308" s="3">
+        <v>148019</v>
+      </c>
+      <c r="G308" s="3">
+        <v>159474</v>
+      </c>
+      <c r="H308" s="3">
+        <v>157564</v>
+      </c>
+      <c r="I308" s="3">
+        <v>161255</v>
+      </c>
+      <c r="J308" s="3">
+        <v>157680</v>
+      </c>
+    </row>
+    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>7</v>
       </c>
@@ -8204,10 +8334,28 @@
       </c>
       <c r="D309" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+        <v>917098</v>
+      </c>
+      <c r="E309" s="3">
+        <v>149370</v>
+      </c>
+      <c r="F309" s="3">
+        <v>157524</v>
+      </c>
+      <c r="G309" s="3">
+        <v>156004</v>
+      </c>
+      <c r="H309" s="3">
+        <v>152274</v>
+      </c>
+      <c r="I309" s="3">
+        <v>148584</v>
+      </c>
+      <c r="J309" s="3">
+        <v>153342</v>
+      </c>
+    </row>
+    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>7</v>
       </c>
@@ -8219,10 +8367,28 @@
       </c>
       <c r="D310" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+        <v>936264</v>
+      </c>
+      <c r="E310" s="3">
+        <v>160964</v>
+      </c>
+      <c r="F310" s="3">
+        <v>155676</v>
+      </c>
+      <c r="G310" s="3">
+        <v>159099</v>
+      </c>
+      <c r="H310" s="3">
+        <v>150479</v>
+      </c>
+      <c r="I310" s="3">
+        <v>151684</v>
+      </c>
+      <c r="J310" s="3">
+        <v>158362</v>
+      </c>
+    </row>
+    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>7</v>
       </c>
@@ -8234,10 +8400,28 @@
       </c>
       <c r="D311" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+        <v>941409</v>
+      </c>
+      <c r="E311" s="3">
+        <v>156352</v>
+      </c>
+      <c r="F311" s="3">
+        <v>155458</v>
+      </c>
+      <c r="G311" s="3">
+        <v>153215</v>
+      </c>
+      <c r="H311" s="3">
+        <v>158029</v>
+      </c>
+      <c r="I311" s="3">
+        <v>161011</v>
+      </c>
+      <c r="J311" s="3">
+        <v>157344</v>
+      </c>
+    </row>
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>7</v>
       </c>
@@ -8249,10 +8433,28 @@
       </c>
       <c r="D312" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+        <v>914710</v>
+      </c>
+      <c r="E312" s="3">
+        <v>151497</v>
+      </c>
+      <c r="F312" s="3">
+        <v>156978</v>
+      </c>
+      <c r="G312" s="3">
+        <v>151806</v>
+      </c>
+      <c r="H312" s="3">
+        <v>149992</v>
+      </c>
+      <c r="I312" s="3">
+        <v>150218</v>
+      </c>
+      <c r="J312" s="3">
+        <v>154219</v>
+      </c>
+    </row>
+    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>7</v>
       </c>
@@ -8264,10 +8466,28 @@
       </c>
       <c r="D313" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+        <v>930790</v>
+      </c>
+      <c r="E313" s="3">
+        <v>160242</v>
+      </c>
+      <c r="F313" s="3">
+        <v>148681</v>
+      </c>
+      <c r="G313" s="3">
+        <v>149423</v>
+      </c>
+      <c r="H313" s="3">
+        <v>156637</v>
+      </c>
+      <c r="I313" s="3">
+        <v>154871</v>
+      </c>
+      <c r="J313" s="3">
+        <v>160936</v>
+      </c>
+    </row>
+    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>7</v>
       </c>
@@ -8279,10 +8499,28 @@
       </c>
       <c r="D314" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+        <v>918802</v>
+      </c>
+      <c r="E314" s="3">
+        <v>157736</v>
+      </c>
+      <c r="F314" s="3">
+        <v>149070</v>
+      </c>
+      <c r="G314" s="3">
+        <v>154291</v>
+      </c>
+      <c r="H314" s="3">
+        <v>148256</v>
+      </c>
+      <c r="I314" s="3">
+        <v>150892</v>
+      </c>
+      <c r="J314" s="3">
+        <v>158557</v>
+      </c>
+    </row>
+    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>7</v>
       </c>
@@ -8294,10 +8532,28 @@
       </c>
       <c r="D315" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+        <v>922717</v>
+      </c>
+      <c r="E315" s="3">
+        <v>150271</v>
+      </c>
+      <c r="F315" s="3">
+        <v>159752</v>
+      </c>
+      <c r="G315" s="3">
+        <v>154253</v>
+      </c>
+      <c r="H315" s="3">
+        <v>151376</v>
+      </c>
+      <c r="I315" s="3">
+        <v>157554</v>
+      </c>
+      <c r="J315" s="3">
+        <v>149511</v>
+      </c>
+    </row>
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>7</v>
       </c>
@@ -8309,10 +8565,28 @@
       </c>
       <c r="D316" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+        <v>922635</v>
+      </c>
+      <c r="E316" s="3">
+        <v>148357</v>
+      </c>
+      <c r="F316" s="3">
+        <v>152008</v>
+      </c>
+      <c r="G316" s="3">
+        <v>152935</v>
+      </c>
+      <c r="H316" s="3">
+        <v>160283</v>
+      </c>
+      <c r="I316" s="3">
+        <v>160979</v>
+      </c>
+      <c r="J316" s="3">
+        <v>148073</v>
+      </c>
+    </row>
+    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>7</v>
       </c>
@@ -8324,10 +8598,28 @@
       </c>
       <c r="D317" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
+        <v>934521</v>
+      </c>
+      <c r="E317" s="3">
+        <v>151033</v>
+      </c>
+      <c r="F317" s="3">
+        <v>157933</v>
+      </c>
+      <c r="G317" s="3">
+        <v>156175</v>
+      </c>
+      <c r="H317" s="3">
+        <v>156164</v>
+      </c>
+      <c r="I317" s="3">
+        <v>152760</v>
+      </c>
+      <c r="J317" s="3">
+        <v>160456</v>
+      </c>
+    </row>
+    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>7</v>
       </c>
@@ -8339,10 +8631,28 @@
       </c>
       <c r="D318" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
+        <v>919312</v>
+      </c>
+      <c r="E318" s="3">
+        <v>151476</v>
+      </c>
+      <c r="F318" s="3">
+        <v>154393</v>
+      </c>
+      <c r="G318" s="3">
+        <v>149645</v>
+      </c>
+      <c r="H318" s="3">
+        <v>161448</v>
+      </c>
+      <c r="I318" s="3">
+        <v>154036</v>
+      </c>
+      <c r="J318" s="3">
+        <v>148314</v>
+      </c>
+    </row>
+    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>7</v>
       </c>
@@ -8354,10 +8664,28 @@
       </c>
       <c r="D319" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
+        <v>934043</v>
+      </c>
+      <c r="E319" s="3">
+        <v>157698</v>
+      </c>
+      <c r="F319" s="3">
+        <v>153526</v>
+      </c>
+      <c r="G319" s="3">
+        <v>161364</v>
+      </c>
+      <c r="H319" s="3">
+        <v>149780</v>
+      </c>
+      <c r="I319" s="3">
+        <v>157933</v>
+      </c>
+      <c r="J319" s="3">
+        <v>153742</v>
+      </c>
+    </row>
+    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>7</v>
       </c>
@@ -8369,10 +8697,28 @@
       </c>
       <c r="D320" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+        <v>932737</v>
+      </c>
+      <c r="E320" s="3">
+        <v>149531</v>
+      </c>
+      <c r="F320" s="3">
+        <v>148230</v>
+      </c>
+      <c r="G320" s="3">
+        <v>161324</v>
+      </c>
+      <c r="H320" s="3">
+        <v>152685</v>
+      </c>
+      <c r="I320" s="3">
+        <v>160522</v>
+      </c>
+      <c r="J320" s="3">
+        <v>160445</v>
+      </c>
+    </row>
+    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>7</v>
       </c>
@@ -8384,10 +8730,28 @@
       </c>
       <c r="D321" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+        <v>922581</v>
+      </c>
+      <c r="E321" s="3">
+        <v>156415</v>
+      </c>
+      <c r="F321" s="3">
+        <v>154196</v>
+      </c>
+      <c r="G321" s="3">
+        <v>148861</v>
+      </c>
+      <c r="H321" s="3">
+        <v>160633</v>
+      </c>
+      <c r="I321" s="3">
+        <v>152437</v>
+      </c>
+      <c r="J321" s="3">
+        <v>150039</v>
+      </c>
+    </row>
+    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>7</v>
       </c>
@@ -8399,10 +8763,28 @@
       </c>
       <c r="D322" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+        <v>930086</v>
+      </c>
+      <c r="E322" s="3">
+        <v>148442</v>
+      </c>
+      <c r="F322" s="3">
+        <v>155009</v>
+      </c>
+      <c r="G322" s="3">
+        <v>161566</v>
+      </c>
+      <c r="H322" s="3">
+        <v>154771</v>
+      </c>
+      <c r="I322" s="3">
+        <v>153698</v>
+      </c>
+      <c r="J322" s="3">
+        <v>156600</v>
+      </c>
+    </row>
+    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>7</v>
       </c>
@@ -8414,10 +8796,28 @@
       </c>
       <c r="D323" s="3">
         <f t="shared" ref="D323:D351" si="5">SUM(E323:J323)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+        <v>940191</v>
+      </c>
+      <c r="E323" s="3">
+        <v>154541</v>
+      </c>
+      <c r="F323" s="3">
+        <v>156599</v>
+      </c>
+      <c r="G323" s="3">
+        <v>158352</v>
+      </c>
+      <c r="H323" s="3">
+        <v>156875</v>
+      </c>
+      <c r="I323" s="3">
+        <v>154690</v>
+      </c>
+      <c r="J323" s="3">
+        <v>159134</v>
+      </c>
+    </row>
+    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>7</v>
       </c>
@@ -8429,10 +8829,28 @@
       </c>
       <c r="D324" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+        <v>928158</v>
+      </c>
+      <c r="E324" s="3">
+        <v>151011</v>
+      </c>
+      <c r="F324" s="3">
+        <v>160866</v>
+      </c>
+      <c r="G324" s="3">
+        <v>154397</v>
+      </c>
+      <c r="H324" s="3">
+        <v>153190</v>
+      </c>
+      <c r="I324" s="3">
+        <v>160095</v>
+      </c>
+      <c r="J324" s="3">
+        <v>148599</v>
+      </c>
+    </row>
+    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>7</v>
       </c>
@@ -8444,10 +8862,28 @@
       </c>
       <c r="D325" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
+        <v>955056</v>
+      </c>
+      <c r="E325" s="3">
+        <v>156962</v>
+      </c>
+      <c r="F325" s="3">
+        <v>160798</v>
+      </c>
+      <c r="G325" s="3">
+        <v>161421</v>
+      </c>
+      <c r="H325" s="3">
+        <v>159997</v>
+      </c>
+      <c r="I325" s="3">
+        <v>157457</v>
+      </c>
+      <c r="J325" s="3">
+        <v>158421</v>
+      </c>
+    </row>
+    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>7</v>
       </c>
@@ -8459,10 +8895,28 @@
       </c>
       <c r="D326" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+        <v>931005</v>
+      </c>
+      <c r="E326" s="3">
+        <v>153998</v>
+      </c>
+      <c r="F326" s="3">
+        <v>148838</v>
+      </c>
+      <c r="G326" s="3">
+        <v>159790</v>
+      </c>
+      <c r="H326" s="3">
+        <v>152521</v>
+      </c>
+      <c r="I326" s="3">
+        <v>159086</v>
+      </c>
+      <c r="J326" s="3">
+        <v>156772</v>
+      </c>
+    </row>
+    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>7</v>
       </c>
@@ -8477,7 +8931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>7</v>
       </c>
@@ -8492,7 +8946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>7</v>
       </c>
@@ -8507,7 +8961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>7</v>
       </c>
@@ -8522,7 +8976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>7</v>
       </c>
@@ -8537,7 +8991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>7</v>
       </c>
@@ -8552,7 +9006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>7</v>
       </c>
@@ -8567,7 +9021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>7</v>
       </c>
@@ -8582,7 +9036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>7</v>
       </c>
@@ -8597,7 +9051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>7</v>
       </c>
@@ -8841,7 +9295,7 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="N2:N6 N7:N8" formulaRange="1"/>
+    <ignoredError sqref="N2:N8" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add final data set for workflow 7
</commit_message>
<xml_diff>
--- a/workflow-analysis-and-rewrite/runtime-analysis-and-rewrite.xlsx
+++ b/workflow-analysis-and-rewrite/runtime-analysis-and-rewrite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wederbn\Desktop\Coding\PlanQK\qprov-content\workflow-analysis-and-rewrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B363ABA-FD63-40D3-A200-ED1776607D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6F0D7F-D8BE-42C9-86E1-DF1BE0AF5109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{DFC69C5A-AAD8-407D-8907-336986DC4050}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="11295" xr2:uid="{DFC69C5A-AAD8-407D-8907-336986DC4050}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4836293F-B9CB-4320-909E-74B95BB4C54A}">
   <dimension ref="A1:O351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A313" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,7 +735,7 @@
       </c>
       <c r="O8">
         <f>MEDIAN(D302:D351)</f>
-        <v>457355</v>
+        <v>929193</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -8928,7 +8928,25 @@
       </c>
       <c r="D327" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>928307</v>
+      </c>
+      <c r="E327" s="3">
+        <v>149259</v>
+      </c>
+      <c r="F327" s="3">
+        <v>159806</v>
+      </c>
+      <c r="G327" s="3">
+        <v>154333</v>
+      </c>
+      <c r="H327" s="3">
+        <v>154281</v>
+      </c>
+      <c r="I327" s="3">
+        <v>151909</v>
+      </c>
+      <c r="J327" s="3">
+        <v>158719</v>
       </c>
     </row>
     <row r="328" spans="1:10" x14ac:dyDescent="0.25">
@@ -8943,7 +8961,25 @@
       </c>
       <c r="D328" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>947842</v>
+      </c>
+      <c r="E328" s="3">
+        <v>160216</v>
+      </c>
+      <c r="F328" s="3">
+        <v>159071</v>
+      </c>
+      <c r="G328" s="3">
+        <v>159982</v>
+      </c>
+      <c r="H328" s="3">
+        <v>151660</v>
+      </c>
+      <c r="I328" s="3">
+        <v>155168</v>
+      </c>
+      <c r="J328" s="3">
+        <v>161745</v>
       </c>
     </row>
     <row r="329" spans="1:10" x14ac:dyDescent="0.25">
@@ -8958,7 +8994,25 @@
       </c>
       <c r="D329" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>938570</v>
+      </c>
+      <c r="E329" s="3">
+        <v>155096</v>
+      </c>
+      <c r="F329" s="3">
+        <v>155892</v>
+      </c>
+      <c r="G329" s="3">
+        <v>159195</v>
+      </c>
+      <c r="H329" s="3">
+        <v>161682</v>
+      </c>
+      <c r="I329" s="3">
+        <v>151608</v>
+      </c>
+      <c r="J329" s="3">
+        <v>155097</v>
       </c>
     </row>
     <row r="330" spans="1:10" x14ac:dyDescent="0.25">
@@ -8973,7 +9027,25 @@
       </c>
       <c r="D330" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>923918</v>
+      </c>
+      <c r="E330" s="3">
+        <v>151339</v>
+      </c>
+      <c r="F330" s="3">
+        <v>150637</v>
+      </c>
+      <c r="G330" s="3">
+        <v>151507</v>
+      </c>
+      <c r="H330" s="3">
+        <v>159123</v>
+      </c>
+      <c r="I330" s="3">
+        <v>156141</v>
+      </c>
+      <c r="J330" s="3">
+        <v>155171</v>
       </c>
     </row>
     <row r="331" spans="1:10" x14ac:dyDescent="0.25">
@@ -8988,7 +9060,25 @@
       </c>
       <c r="D331" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>925961</v>
+      </c>
+      <c r="E331" s="3">
+        <v>155159</v>
+      </c>
+      <c r="F331" s="3">
+        <v>154328</v>
+      </c>
+      <c r="G331" s="3">
+        <v>158971</v>
+      </c>
+      <c r="H331" s="3">
+        <v>149918</v>
+      </c>
+      <c r="I331" s="3">
+        <v>158024</v>
+      </c>
+      <c r="J331" s="3">
+        <v>149561</v>
       </c>
     </row>
     <row r="332" spans="1:10" x14ac:dyDescent="0.25">
@@ -9003,7 +9093,25 @@
       </c>
       <c r="D332" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>924431</v>
+      </c>
+      <c r="E332" s="3">
+        <v>156713</v>
+      </c>
+      <c r="F332" s="3">
+        <v>151664</v>
+      </c>
+      <c r="G332" s="3">
+        <v>156271</v>
+      </c>
+      <c r="H332" s="3">
+        <v>148155</v>
+      </c>
+      <c r="I332" s="3">
+        <v>152090</v>
+      </c>
+      <c r="J332" s="3">
+        <v>159538</v>
       </c>
     </row>
     <row r="333" spans="1:10" x14ac:dyDescent="0.25">
@@ -9018,7 +9126,25 @@
       </c>
       <c r="D333" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>921815</v>
+      </c>
+      <c r="E333" s="3">
+        <v>152646</v>
+      </c>
+      <c r="F333" s="3">
+        <v>148195</v>
+      </c>
+      <c r="G333" s="3">
+        <v>151259</v>
+      </c>
+      <c r="H333" s="3">
+        <v>158289</v>
+      </c>
+      <c r="I333" s="3">
+        <v>154263</v>
+      </c>
+      <c r="J333" s="3">
+        <v>157163</v>
       </c>
     </row>
     <row r="334" spans="1:10" x14ac:dyDescent="0.25">
@@ -9033,7 +9159,25 @@
       </c>
       <c r="D334" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>930715</v>
+      </c>
+      <c r="E334" s="3">
+        <v>150416</v>
+      </c>
+      <c r="F334" s="3">
+        <v>153587</v>
+      </c>
+      <c r="G334" s="3">
+        <v>160497</v>
+      </c>
+      <c r="H334" s="3">
+        <v>157690</v>
+      </c>
+      <c r="I334" s="3">
+        <v>156956</v>
+      </c>
+      <c r="J334" s="3">
+        <v>151569</v>
       </c>
     </row>
     <row r="335" spans="1:10" x14ac:dyDescent="0.25">
@@ -9048,7 +9192,25 @@
       </c>
       <c r="D335" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>918201</v>
+      </c>
+      <c r="E335" s="3">
+        <v>150558</v>
+      </c>
+      <c r="F335" s="3">
+        <v>153484</v>
+      </c>
+      <c r="G335" s="3">
+        <v>151469</v>
+      </c>
+      <c r="H335" s="3">
+        <v>157312</v>
+      </c>
+      <c r="I335" s="3">
+        <v>152320</v>
+      </c>
+      <c r="J335" s="3">
+        <v>153058</v>
       </c>
     </row>
     <row r="336" spans="1:10" x14ac:dyDescent="0.25">
@@ -9063,10 +9225,28 @@
       </c>
       <c r="D336" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+        <v>941138</v>
+      </c>
+      <c r="E336" s="3">
+        <v>160636</v>
+      </c>
+      <c r="F336" s="3">
+        <v>155126</v>
+      </c>
+      <c r="G336" s="3">
+        <v>150385</v>
+      </c>
+      <c r="H336" s="3">
+        <v>155922</v>
+      </c>
+      <c r="I336" s="3">
+        <v>157596</v>
+      </c>
+      <c r="J336" s="3">
+        <v>161473</v>
+      </c>
+    </row>
+    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>7</v>
       </c>
@@ -9078,10 +9258,28 @@
       </c>
       <c r="D337" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+        <v>929746</v>
+      </c>
+      <c r="E337" s="3">
+        <v>150645</v>
+      </c>
+      <c r="F337" s="3">
+        <v>159451</v>
+      </c>
+      <c r="G337" s="3">
+        <v>150554</v>
+      </c>
+      <c r="H337" s="3">
+        <v>153991</v>
+      </c>
+      <c r="I337" s="3">
+        <v>153751</v>
+      </c>
+      <c r="J337" s="3">
+        <v>161354</v>
+      </c>
+    </row>
+    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>7</v>
       </c>
@@ -9093,10 +9291,28 @@
       </c>
       <c r="D338" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+        <v>926531</v>
+      </c>
+      <c r="E338" s="3">
+        <v>156562</v>
+      </c>
+      <c r="F338" s="3">
+        <v>153898</v>
+      </c>
+      <c r="G338" s="3">
+        <v>151209</v>
+      </c>
+      <c r="H338" s="3">
+        <v>148625</v>
+      </c>
+      <c r="I338" s="3">
+        <v>157186</v>
+      </c>
+      <c r="J338" s="3">
+        <v>159051</v>
+      </c>
+    </row>
+    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>7</v>
       </c>
@@ -9108,10 +9324,28 @@
       </c>
       <c r="D339" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+        <v>924451</v>
+      </c>
+      <c r="E339" s="3">
+        <v>152697</v>
+      </c>
+      <c r="F339" s="3">
+        <v>148624</v>
+      </c>
+      <c r="G339" s="3">
+        <v>154348</v>
+      </c>
+      <c r="H339" s="3">
+        <v>155957</v>
+      </c>
+      <c r="I339" s="3">
+        <v>161553</v>
+      </c>
+      <c r="J339" s="3">
+        <v>151272</v>
+      </c>
+    </row>
+    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>7</v>
       </c>
@@ -9123,10 +9357,28 @@
       </c>
       <c r="D340" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+        <v>929651</v>
+      </c>
+      <c r="E340" s="3">
+        <v>159805</v>
+      </c>
+      <c r="F340" s="3">
+        <v>158494</v>
+      </c>
+      <c r="G340" s="3">
+        <v>149645</v>
+      </c>
+      <c r="H340" s="3">
+        <v>157835</v>
+      </c>
+      <c r="I340" s="3">
+        <v>155737</v>
+      </c>
+      <c r="J340" s="3">
+        <v>148135</v>
+      </c>
+    </row>
+    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>7</v>
       </c>
@@ -9138,10 +9390,28 @@
       </c>
       <c r="D341" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+        <v>912184</v>
+      </c>
+      <c r="E341" s="3">
+        <v>151137</v>
+      </c>
+      <c r="F341" s="3">
+        <v>153214</v>
+      </c>
+      <c r="G341" s="3">
+        <v>150485</v>
+      </c>
+      <c r="H341" s="3">
+        <v>149302</v>
+      </c>
+      <c r="I341" s="3">
+        <v>155232</v>
+      </c>
+      <c r="J341" s="3">
+        <v>152814</v>
+      </c>
+    </row>
+    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>7</v>
       </c>
@@ -9153,10 +9423,28 @@
       </c>
       <c r="D342" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
+        <v>921193</v>
+      </c>
+      <c r="E342" s="3">
+        <v>154038</v>
+      </c>
+      <c r="F342" s="3">
+        <v>148593</v>
+      </c>
+      <c r="G342" s="3">
+        <v>154376</v>
+      </c>
+      <c r="H342" s="3">
+        <v>149363</v>
+      </c>
+      <c r="I342" s="3">
+        <v>158208</v>
+      </c>
+      <c r="J342" s="3">
+        <v>156615</v>
+      </c>
+    </row>
+    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>7</v>
       </c>
@@ -9168,10 +9456,28 @@
       </c>
       <c r="D343" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
+        <v>922913</v>
+      </c>
+      <c r="E343" s="3">
+        <v>150410</v>
+      </c>
+      <c r="F343" s="3">
+        <v>153397</v>
+      </c>
+      <c r="G343" s="3">
+        <v>161361</v>
+      </c>
+      <c r="H343" s="3">
+        <v>151654</v>
+      </c>
+      <c r="I343" s="3">
+        <v>149936</v>
+      </c>
+      <c r="J343" s="3">
+        <v>156155</v>
+      </c>
+    </row>
+    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>7</v>
       </c>
@@ -9183,10 +9489,28 @@
       </c>
       <c r="D344" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
+        <v>935749</v>
+      </c>
+      <c r="E344" s="3">
+        <v>154457</v>
+      </c>
+      <c r="F344" s="3">
+        <v>159251</v>
+      </c>
+      <c r="G344" s="3">
+        <v>154559</v>
+      </c>
+      <c r="H344" s="3">
+        <v>157733</v>
+      </c>
+      <c r="I344" s="3">
+        <v>156178</v>
+      </c>
+      <c r="J344" s="3">
+        <v>153571</v>
+      </c>
+    </row>
+    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>7</v>
       </c>
@@ -9198,10 +9522,28 @@
       </c>
       <c r="D345" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
+        <v>938478</v>
+      </c>
+      <c r="E345" s="3">
+        <v>148663</v>
+      </c>
+      <c r="F345" s="3">
+        <v>160185</v>
+      </c>
+      <c r="G345" s="3">
+        <v>157611</v>
+      </c>
+      <c r="H345" s="3">
+        <v>158705</v>
+      </c>
+      <c r="I345" s="3">
+        <v>156744</v>
+      </c>
+      <c r="J345" s="3">
+        <v>156570</v>
+      </c>
+    </row>
+    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>7</v>
       </c>
@@ -9213,10 +9555,28 @@
       </c>
       <c r="D346" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
+        <v>946633</v>
+      </c>
+      <c r="E346" s="3">
+        <v>161155</v>
+      </c>
+      <c r="F346" s="3">
+        <v>160133</v>
+      </c>
+      <c r="G346" s="3">
+        <v>152867</v>
+      </c>
+      <c r="H346" s="3">
+        <v>152467</v>
+      </c>
+      <c r="I346" s="3">
+        <v>159315</v>
+      </c>
+      <c r="J346" s="3">
+        <v>160696</v>
+      </c>
+    </row>
+    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>7</v>
       </c>
@@ -9228,10 +9588,28 @@
       </c>
       <c r="D347" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
+        <v>930308</v>
+      </c>
+      <c r="E347" s="3">
+        <v>156139</v>
+      </c>
+      <c r="F347" s="3">
+        <v>159442</v>
+      </c>
+      <c r="G347" s="3">
+        <v>149280</v>
+      </c>
+      <c r="H347" s="3">
+        <v>158300</v>
+      </c>
+      <c r="I347" s="3">
+        <v>156599</v>
+      </c>
+      <c r="J347" s="3">
+        <v>150548</v>
+      </c>
+    </row>
+    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>7</v>
       </c>
@@ -9243,10 +9621,28 @@
       </c>
       <c r="D348" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
+        <v>927690</v>
+      </c>
+      <c r="E348" s="3">
+        <v>161378</v>
+      </c>
+      <c r="F348" s="3">
+        <v>149368</v>
+      </c>
+      <c r="G348" s="3">
+        <v>155626</v>
+      </c>
+      <c r="H348" s="3">
+        <v>149459</v>
+      </c>
+      <c r="I348" s="3">
+        <v>160088</v>
+      </c>
+      <c r="J348" s="3">
+        <v>151771</v>
+      </c>
+    </row>
+    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>7</v>
       </c>
@@ -9258,10 +9654,28 @@
       </c>
       <c r="D349" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
+        <v>912060</v>
+      </c>
+      <c r="E349" s="3">
+        <v>152869</v>
+      </c>
+      <c r="F349" s="3">
+        <v>151286</v>
+      </c>
+      <c r="G349" s="3">
+        <v>150760</v>
+      </c>
+      <c r="H349" s="3">
+        <v>154107</v>
+      </c>
+      <c r="I349" s="3">
+        <v>153650</v>
+      </c>
+      <c r="J349" s="3">
+        <v>149388</v>
+      </c>
+    </row>
+    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>7</v>
       </c>
@@ -9273,10 +9687,28 @@
       </c>
       <c r="D350" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
+        <v>913334</v>
+      </c>
+      <c r="E350" s="3">
+        <v>148842</v>
+      </c>
+      <c r="F350" s="3">
+        <v>151933</v>
+      </c>
+      <c r="G350" s="3">
+        <v>151485</v>
+      </c>
+      <c r="H350" s="3">
+        <v>155333</v>
+      </c>
+      <c r="I350" s="3">
+        <v>150901</v>
+      </c>
+      <c r="J350" s="3">
+        <v>154840</v>
+      </c>
+    </row>
+    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>7</v>
       </c>
@@ -9288,7 +9720,25 @@
       </c>
       <c r="D351" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>928735</v>
+      </c>
+      <c r="E351" s="3">
+        <v>159202</v>
+      </c>
+      <c r="F351" s="3">
+        <v>158282</v>
+      </c>
+      <c r="G351" s="3">
+        <v>151242</v>
+      </c>
+      <c r="H351" s="3">
+        <v>150645</v>
+      </c>
+      <c r="I351" s="3">
+        <v>152393</v>
+      </c>
+      <c r="J351" s="3">
+        <v>156971</v>
       </c>
     </row>
   </sheetData>

</xml_diff>